<commit_message>
Setup migration for old surveys
</commit_message>
<xml_diff>
--- a/data_dict.xlsx
+++ b/data_dict.xlsx
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="tabla-survey" sheetId="1" r:id="rId1"/>
     <sheet name="tabla-locations" sheetId="2" r:id="rId2"/>
+    <sheet name="tabla-summary" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="283">
   <si>
     <t>Pregunta</t>
   </si>
@@ -782,9 +783,6 @@
     <t>Estampilla de tiempo en milisegundos de la actividad registrada</t>
   </si>
   <si>
-    <t>Se toma desde el primero de Enero 1 de 1970</t>
-  </si>
-  <si>
     <t>activity</t>
   </si>
   <si>
@@ -803,9 +801,6 @@
     <t>Id del entrevistado</t>
   </si>
   <si>
-    <t>Debe coincidir con el de la tabla: "survey prod"</t>
-  </si>
-  <si>
     <t>vertical_accuracy</t>
   </si>
   <si>
@@ -822,9 +817,6 @@
   </si>
   <si>
     <t>TINYINT - UNSIGNED</t>
-  </si>
-  <si>
-    <t>Se toma desde  Enero 1 del 2000</t>
   </si>
   <si>
     <t xml:space="preserve">Estampilla de tiempo en segundos </t>
@@ -847,7 +839,82 @@
  "WALKING" : "WAL"</t>
   </si>
   <si>
-    <t>VARCHAR(12) - NOT NULL</t>
+    <t>Debe coincidir con el de la tabla: "survey prod". Ya se encuentra anonimizado</t>
+  </si>
+  <si>
+    <t>Ya se encuentra anonimizado</t>
+  </si>
+  <si>
+    <t>Se toma desde  Enero 1 del 2000 (Basta con sumarle 946684800 segundos)</t>
+  </si>
+  <si>
+    <t>Diccionario de datos para la taba: "summary_prod"</t>
+  </si>
+  <si>
+    <t>Carnet del entrevistado</t>
+  </si>
+  <si>
+    <t>Debe coincidir con el de la tabla: "survey prod"</t>
+  </si>
+  <si>
+    <t>timestamp_json</t>
+  </si>
+  <si>
+    <t>BIGINT - UNSIGNED</t>
+  </si>
+  <si>
+    <t>json_id</t>
+  </si>
+  <si>
+    <t>CHAR(32)</t>
+  </si>
+  <si>
+    <t>entrego_json</t>
+  </si>
+  <si>
+    <t>Estampilla de tiempo en segundos de la hora que entrego el JSON</t>
+  </si>
+  <si>
+    <t>Identificador de hash del JSON</t>
+  </si>
+  <si>
+    <t>Indica si ya se entrego el JSON o no</t>
+  </si>
+  <si>
+    <t>BOOLEAN</t>
+  </si>
+  <si>
+    <t>timestamp_encuesta</t>
+  </si>
+  <si>
+    <t>Se toma desde  Enero 1 del 1970</t>
+  </si>
+  <si>
+    <t>Estampilla de tiempo en segundos de la hora que entrego la encuesta</t>
+  </si>
+  <si>
+    <t>grupo</t>
+  </si>
+  <si>
+    <t>Grupo al cual pertenece el entrevistado</t>
+  </si>
+  <si>
+    <t>VARCHAR(25)</t>
+  </si>
+  <si>
+    <t>entrego_encuesta</t>
+  </si>
+  <si>
+    <t>Indica si ya se entrego la encuesta o no</t>
+  </si>
+  <si>
+    <t>exporto_json</t>
+  </si>
+  <si>
+    <t>Indica si ya se exporto el JSON o no a la base de datos</t>
+  </si>
+  <si>
+    <t>VARCHAR(18) - NOT NULL</t>
   </si>
 </sst>
 </file>
@@ -1139,7 +1206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1209,6 +1276,81 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1239,80 +1381,17 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1593,7 +1672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -1603,26 +1682,26 @@
     <col min="2" max="2" width="45.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="32.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="31.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="31.83203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="68" t="s">
         <v>221</v>
       </c>
-      <c r="B1" s="43"/>
+      <c r="B1" s="68"/>
     </row>
     <row r="2" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
       <c r="E2" s="24" t="s">
         <v>207</v>
       </c>
@@ -1634,46 +1713,48 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
       <c r="E3" s="3"/>
       <c r="F3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="54"/>
-      <c r="B4" s="59" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" s="60"/>
+      <c r="B4" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="3"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="43" t="s">
+        <v>258</v>
+      </c>
       <c r="F4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="G4" s="27" t="s">
-        <v>260</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
       <c r="E5" s="6"/>
       <c r="F5" s="7" t="s">
         <v>9</v>
@@ -1683,12 +1764,12 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="55"/>
-      <c r="B6" s="53" t="s">
+      <c r="A6" s="48"/>
+      <c r="B6" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
       <c r="E6" s="6"/>
       <c r="F6" s="7" t="s">
         <v>10</v>
@@ -1698,12 +1779,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="55"/>
-      <c r="B7" s="53" t="s">
+      <c r="A7" s="48"/>
+      <c r="B7" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
       <c r="E7" s="6"/>
       <c r="F7" s="7" t="s">
         <v>13</v>
@@ -1713,12 +1794,12 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="55"/>
-      <c r="B8" s="53" t="s">
+      <c r="A8" s="48"/>
+      <c r="B8" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
       <c r="E8" s="6"/>
       <c r="F8" s="7" t="s">
         <v>15</v>
@@ -1728,12 +1809,12 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="55"/>
-      <c r="B9" s="53" t="s">
+      <c r="A9" s="48"/>
+      <c r="B9" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
       <c r="E9" s="6"/>
       <c r="F9" s="7" t="s">
         <v>17</v>
@@ -1743,12 +1824,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="55"/>
-      <c r="B10" s="53" t="s">
+      <c r="A10" s="48"/>
+      <c r="B10" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
       <c r="E10" s="6"/>
       <c r="F10" s="7" t="s">
         <v>19</v>
@@ -1758,12 +1839,12 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="55"/>
-      <c r="B11" s="53" t="s">
+      <c r="A11" s="48"/>
+      <c r="B11" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
       <c r="E11" s="6"/>
       <c r="F11" s="7" t="s">
         <v>21</v>
@@ -1773,12 +1854,12 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="55"/>
-      <c r="B12" s="53" t="s">
+      <c r="A12" s="48"/>
+      <c r="B12" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
       <c r="E12" s="6"/>
       <c r="F12" s="7" t="s">
         <v>23</v>
@@ -1788,12 +1869,12 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="55"/>
-      <c r="B13" s="53" t="s">
+      <c r="A13" s="48"/>
+      <c r="B13" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
       <c r="E13" s="6"/>
       <c r="F13" s="7" t="s">
         <v>25</v>
@@ -1803,12 +1884,12 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="55"/>
-      <c r="B14" s="53" t="s">
+      <c r="A14" s="48"/>
+      <c r="B14" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
       <c r="E14" s="6"/>
       <c r="F14" s="7" t="s">
         <v>27</v>
@@ -1818,14 +1899,14 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="56" t="s">
+      <c r="A15" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="57" t="s">
+      <c r="B15" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
       <c r="E15" s="8"/>
       <c r="F15" s="9" t="s">
         <v>30</v>
@@ -1835,12 +1916,12 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="56"/>
-      <c r="B16" s="57" t="s">
+      <c r="A16" s="58"/>
+      <c r="B16" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
       <c r="E16" s="8"/>
       <c r="F16" s="9" t="s">
         <v>32</v>
@@ -1850,12 +1931,12 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="56"/>
-      <c r="B17" s="57" t="s">
+      <c r="A17" s="58"/>
+      <c r="B17" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
       <c r="E17" s="8"/>
       <c r="F17" s="9" t="s">
         <v>34</v>
@@ -1865,12 +1946,12 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="56"/>
-      <c r="B18" s="57" t="s">
+      <c r="A18" s="58"/>
+      <c r="B18" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="54"/>
       <c r="E18" s="8"/>
       <c r="F18" s="9" t="s">
         <v>36</v>
@@ -1880,12 +1961,12 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="56"/>
-      <c r="B19" s="57" t="s">
+      <c r="A19" s="58"/>
+      <c r="B19" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
       <c r="E19" s="8"/>
       <c r="F19" s="9" t="s">
         <v>38</v>
@@ -1895,13 +1976,13 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="60" t="s">
+      <c r="A20" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="61" t="s">
+      <c r="B20" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="61"/>
+      <c r="C20" s="67"/>
       <c r="D20" s="10" t="s">
         <v>43</v>
       </c>
@@ -1914,9 +1995,9 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="60"/>
-      <c r="B21" s="61"/>
-      <c r="C21" s="61"/>
+      <c r="A21" s="66"/>
+      <c r="B21" s="67"/>
+      <c r="C21" s="67"/>
       <c r="D21" s="11" t="s">
         <v>45</v>
       </c>
@@ -1929,9 +2010,9 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="60"/>
-      <c r="B22" s="61"/>
-      <c r="C22" s="61"/>
+      <c r="A22" s="66"/>
+      <c r="B22" s="67"/>
+      <c r="C22" s="67"/>
       <c r="D22" s="11" t="s">
         <v>46</v>
       </c>
@@ -1944,9 +2025,9 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="60"/>
-      <c r="B23" s="61"/>
-      <c r="C23" s="61"/>
+      <c r="A23" s="66"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="67"/>
       <c r="D23" s="11" t="s">
         <v>48</v>
       </c>
@@ -1959,9 +2040,9 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="60"/>
-      <c r="B24" s="61"/>
-      <c r="C24" s="61"/>
+      <c r="A24" s="66"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="67"/>
       <c r="D24" s="11" t="s">
         <v>50</v>
       </c>
@@ -1974,13 +2055,13 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="50" t="s">
+      <c r="A25" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="62" t="s">
+      <c r="B25" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="62"/>
+      <c r="C25" s="61"/>
       <c r="D25" s="13" t="s">
         <v>64</v>
       </c>
@@ -1993,9 +2074,9 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="51"/>
-      <c r="B26" s="62"/>
-      <c r="C26" s="62"/>
+      <c r="A26" s="76"/>
+      <c r="B26" s="61"/>
+      <c r="C26" s="61"/>
       <c r="D26" s="13" t="s">
         <v>67</v>
       </c>
@@ -2008,9 +2089,9 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="51"/>
-      <c r="B27" s="62"/>
-      <c r="C27" s="62"/>
+      <c r="A27" s="76"/>
+      <c r="B27" s="61"/>
+      <c r="C27" s="61"/>
       <c r="D27" s="13" t="s">
         <v>68</v>
       </c>
@@ -2023,9 +2104,9 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="51"/>
-      <c r="B28" s="62"/>
-      <c r="C28" s="62"/>
+      <c r="A28" s="76"/>
+      <c r="B28" s="61"/>
+      <c r="C28" s="61"/>
       <c r="D28" s="13" t="s">
         <v>70</v>
       </c>
@@ -2038,9 +2119,9 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="51"/>
-      <c r="B29" s="62"/>
-      <c r="C29" s="62"/>
+      <c r="A29" s="76"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="61"/>
       <c r="D29" s="13" t="s">
         <v>72</v>
       </c>
@@ -2053,11 +2134,11 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="51"/>
-      <c r="B30" s="62" t="s">
+      <c r="A30" s="76"/>
+      <c r="B30" s="61" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="62"/>
+      <c r="C30" s="61"/>
       <c r="D30" s="13" t="s">
         <v>54</v>
       </c>
@@ -2070,9 +2151,9 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="51"/>
-      <c r="B31" s="62"/>
-      <c r="C31" s="62"/>
+      <c r="A31" s="76"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="61"/>
       <c r="D31" s="13" t="s">
         <v>56</v>
       </c>
@@ -2085,9 +2166,9 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="51"/>
-      <c r="B32" s="62"/>
-      <c r="C32" s="62"/>
+      <c r="A32" s="76"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="61"/>
       <c r="D32" s="13" t="s">
         <v>58</v>
       </c>
@@ -2100,9 +2181,9 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="51"/>
-      <c r="B33" s="62"/>
-      <c r="C33" s="62"/>
+      <c r="A33" s="76"/>
+      <c r="B33" s="61"/>
+      <c r="C33" s="61"/>
       <c r="D33" s="13" t="s">
         <v>60</v>
       </c>
@@ -2115,9 +2196,9 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="51"/>
-      <c r="B34" s="62"/>
-      <c r="C34" s="62"/>
+      <c r="A34" s="76"/>
+      <c r="B34" s="61"/>
+      <c r="C34" s="61"/>
       <c r="D34" s="13" t="s">
         <v>62</v>
       </c>
@@ -2130,12 +2211,12 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="51"/>
-      <c r="B35" s="47" t="s">
+      <c r="A35" s="76"/>
+      <c r="B35" s="72" t="s">
         <v>215</v>
       </c>
-      <c r="C35" s="48"/>
-      <c r="D35" s="49"/>
+      <c r="C35" s="73"/>
+      <c r="D35" s="74"/>
       <c r="E35" s="13"/>
       <c r="F35" s="14" t="s">
         <v>216</v>
@@ -2145,12 +2226,12 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="51"/>
-      <c r="B36" s="47" t="s">
+      <c r="A36" s="76"/>
+      <c r="B36" s="72" t="s">
         <v>217</v>
       </c>
-      <c r="C36" s="48"/>
-      <c r="D36" s="49"/>
+      <c r="C36" s="73"/>
+      <c r="D36" s="74"/>
       <c r="E36" s="13"/>
       <c r="F36" s="14" t="s">
         <v>218</v>
@@ -2160,12 +2241,12 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="52"/>
-      <c r="B37" s="47" t="s">
+      <c r="A37" s="77"/>
+      <c r="B37" s="72" t="s">
         <v>219</v>
       </c>
-      <c r="C37" s="48"/>
-      <c r="D37" s="49"/>
+      <c r="C37" s="73"/>
+      <c r="D37" s="74"/>
       <c r="E37" s="13"/>
       <c r="F37" s="14" t="s">
         <v>220</v>
@@ -2175,14 +2256,14 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="58" t="s">
+      <c r="A38" s="78" t="s">
         <v>75</v>
       </c>
-      <c r="B38" s="44" t="s">
+      <c r="B38" s="69" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="45"/>
-      <c r="D38" s="46"/>
+      <c r="C38" s="70"/>
+      <c r="D38" s="71"/>
       <c r="E38" s="15"/>
       <c r="F38" s="18" t="s">
         <v>77</v>
@@ -2192,12 +2273,12 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="58"/>
-      <c r="B39" s="64" t="s">
+      <c r="A39" s="78"/>
+      <c r="B39" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="C39" s="64"/>
-      <c r="D39" s="64"/>
+      <c r="C39" s="62"/>
+      <c r="D39" s="62"/>
       <c r="E39" s="16"/>
       <c r="F39" s="18" t="s">
         <v>79</v>
@@ -2207,12 +2288,12 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="58"/>
-      <c r="B40" s="64" t="s">
+      <c r="A40" s="78"/>
+      <c r="B40" s="62" t="s">
         <v>80</v>
       </c>
-      <c r="C40" s="64"/>
-      <c r="D40" s="64"/>
+      <c r="C40" s="62"/>
+      <c r="D40" s="62"/>
       <c r="E40" s="16"/>
       <c r="F40" s="18" t="s">
         <v>81</v>
@@ -2222,11 +2303,11 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="58"/>
-      <c r="B41" s="65" t="s">
+      <c r="A41" s="78"/>
+      <c r="B41" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="C41" s="65"/>
+      <c r="C41" s="63"/>
       <c r="D41" s="17" t="s">
         <v>24</v>
       </c>
@@ -2239,9 +2320,9 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="58"/>
-      <c r="B42" s="65"/>
-      <c r="C42" s="65"/>
+      <c r="A42" s="78"/>
+      <c r="B42" s="63"/>
+      <c r="C42" s="63"/>
       <c r="D42" s="17" t="s">
         <v>83</v>
       </c>
@@ -2254,9 +2335,9 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="58"/>
-      <c r="B43" s="65"/>
-      <c r="C43" s="65"/>
+      <c r="A43" s="78"/>
+      <c r="B43" s="63"/>
+      <c r="C43" s="63"/>
       <c r="D43" s="17" t="s">
         <v>84</v>
       </c>
@@ -2269,14 +2350,14 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="76" t="s">
+      <c r="A44" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="B44" s="67" t="s">
+      <c r="B44" s="65" t="s">
         <v>89</v>
       </c>
-      <c r="C44" s="67"/>
-      <c r="D44" s="67"/>
+      <c r="C44" s="65"/>
+      <c r="D44" s="65"/>
       <c r="E44" s="19"/>
       <c r="F44" s="21" t="s">
         <v>90</v>
@@ -2286,12 +2367,12 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="76"/>
-      <c r="B45" s="66" t="s">
+      <c r="A45" s="52"/>
+      <c r="B45" s="64" t="s">
         <v>91</v>
       </c>
-      <c r="C45" s="66"/>
-      <c r="D45" s="66"/>
+      <c r="C45" s="64"/>
+      <c r="D45" s="64"/>
       <c r="E45" s="20"/>
       <c r="F45" s="21" t="s">
         <v>92</v>
@@ -2301,17 +2382,17 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="54" t="s">
+      <c r="A46" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="B46" s="63" t="s">
+      <c r="B46" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="C46" s="63"/>
+      <c r="C46" s="53"/>
       <c r="D46" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="E46" s="68" t="s">
+      <c r="E46" s="55" t="s">
         <v>103</v>
       </c>
       <c r="F46" s="5" t="s">
@@ -2322,13 +2403,13 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="54"/>
-      <c r="B47" s="63"/>
-      <c r="C47" s="63"/>
+      <c r="A47" s="60"/>
+      <c r="B47" s="53"/>
+      <c r="C47" s="53"/>
       <c r="D47" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="E47" s="69"/>
+      <c r="E47" s="56"/>
       <c r="F47" s="5" t="s">
         <v>100</v>
       </c>
@@ -2337,13 +2418,13 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="54"/>
-      <c r="B48" s="63"/>
-      <c r="C48" s="63"/>
+      <c r="A48" s="60"/>
+      <c r="B48" s="53"/>
+      <c r="C48" s="53"/>
       <c r="D48" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="E48" s="69"/>
+      <c r="E48" s="56"/>
       <c r="F48" s="5" t="s">
         <v>101</v>
       </c>
@@ -2352,13 +2433,13 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="54"/>
-      <c r="B49" s="63"/>
-      <c r="C49" s="63"/>
+      <c r="A49" s="60"/>
+      <c r="B49" s="53"/>
+      <c r="C49" s="53"/>
       <c r="D49" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="E49" s="70"/>
+      <c r="E49" s="57"/>
       <c r="F49" s="5" t="s">
         <v>102</v>
       </c>
@@ -2367,11 +2448,11 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="54"/>
-      <c r="B50" s="63" t="s">
+      <c r="A50" s="60"/>
+      <c r="B50" s="53" t="s">
         <v>104</v>
       </c>
-      <c r="C50" s="63"/>
+      <c r="C50" s="53"/>
       <c r="D50" s="22" t="s">
         <v>105</v>
       </c>
@@ -2384,9 +2465,9 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="54"/>
-      <c r="B51" s="63"/>
-      <c r="C51" s="63"/>
+      <c r="A51" s="60"/>
+      <c r="B51" s="53"/>
+      <c r="C51" s="53"/>
       <c r="D51" s="22" t="s">
         <v>106</v>
       </c>
@@ -2399,9 +2480,9 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="54"/>
-      <c r="B52" s="63"/>
-      <c r="C52" s="63"/>
+      <c r="A52" s="60"/>
+      <c r="B52" s="53"/>
+      <c r="C52" s="53"/>
       <c r="D52" s="22" t="s">
         <v>107</v>
       </c>
@@ -2414,9 +2495,9 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="54"/>
-      <c r="B53" s="63"/>
-      <c r="C53" s="63"/>
+      <c r="A53" s="60"/>
+      <c r="B53" s="53"/>
+      <c r="C53" s="53"/>
       <c r="D53" s="22" t="s">
         <v>108</v>
       </c>
@@ -2429,9 +2510,9 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" s="54"/>
-      <c r="B54" s="63"/>
-      <c r="C54" s="63"/>
+      <c r="A54" s="60"/>
+      <c r="B54" s="53"/>
+      <c r="C54" s="53"/>
       <c r="D54" s="22" t="s">
         <v>109</v>
       </c>
@@ -2444,9 +2525,9 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="54"/>
-      <c r="B55" s="63"/>
-      <c r="C55" s="63"/>
+      <c r="A55" s="60"/>
+      <c r="B55" s="53"/>
+      <c r="C55" s="53"/>
       <c r="D55" s="22" t="s">
         <v>110</v>
       </c>
@@ -2459,9 +2540,9 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="54"/>
-      <c r="B56" s="63"/>
-      <c r="C56" s="63"/>
+      <c r="A56" s="60"/>
+      <c r="B56" s="53"/>
+      <c r="C56" s="53"/>
       <c r="D56" s="22" t="s">
         <v>111</v>
       </c>
@@ -2474,9 +2555,9 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="54"/>
-      <c r="B57" s="63"/>
-      <c r="C57" s="63"/>
+      <c r="A57" s="60"/>
+      <c r="B57" s="53"/>
+      <c r="C57" s="53"/>
       <c r="D57" s="22" t="s">
         <v>112</v>
       </c>
@@ -2489,14 +2570,14 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="55" t="s">
+      <c r="A58" s="48" t="s">
         <v>121</v>
       </c>
-      <c r="B58" s="53" t="s">
+      <c r="B58" s="50" t="s">
         <v>122</v>
       </c>
-      <c r="C58" s="53"/>
-      <c r="D58" s="53"/>
+      <c r="C58" s="50"/>
+      <c r="D58" s="50"/>
       <c r="E58" s="6"/>
       <c r="F58" s="35" t="s">
         <v>123</v>
@@ -2506,12 +2587,12 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="55"/>
-      <c r="B59" s="53" t="s">
+      <c r="A59" s="48"/>
+      <c r="B59" s="50" t="s">
         <v>125</v>
       </c>
-      <c r="C59" s="53"/>
-      <c r="D59" s="53"/>
+      <c r="C59" s="50"/>
+      <c r="D59" s="50"/>
       <c r="E59" s="6"/>
       <c r="F59" s="35" t="s">
         <v>124</v>
@@ -2521,11 +2602,11 @@
       </c>
     </row>
     <row r="60" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="55"/>
-      <c r="B60" s="72" t="s">
+      <c r="A60" s="48"/>
+      <c r="B60" s="59" t="s">
         <v>126</v>
       </c>
-      <c r="C60" s="73" t="s">
+      <c r="C60" s="51" t="s">
         <v>127</v>
       </c>
       <c r="D60" s="36" t="s">
@@ -2540,9 +2621,9 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" s="55"/>
-      <c r="B61" s="72"/>
-      <c r="C61" s="73"/>
+      <c r="A61" s="48"/>
+      <c r="B61" s="59"/>
+      <c r="C61" s="51"/>
       <c r="D61" s="36" t="s">
         <v>129</v>
       </c>
@@ -2555,9 +2636,9 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" s="55"/>
-      <c r="B62" s="72"/>
-      <c r="C62" s="73"/>
+      <c r="A62" s="48"/>
+      <c r="B62" s="59"/>
+      <c r="C62" s="51"/>
       <c r="D62" s="36" t="s">
         <v>130</v>
       </c>
@@ -2570,9 +2651,9 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="55"/>
-      <c r="B63" s="72"/>
-      <c r="C63" s="73"/>
+      <c r="A63" s="48"/>
+      <c r="B63" s="59"/>
+      <c r="C63" s="51"/>
       <c r="D63" s="36" t="s">
         <v>131</v>
       </c>
@@ -2585,9 +2666,9 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" s="55"/>
-      <c r="B64" s="72"/>
-      <c r="C64" s="73"/>
+      <c r="A64" s="48"/>
+      <c r="B64" s="59"/>
+      <c r="C64" s="51"/>
       <c r="D64" s="36" t="s">
         <v>132</v>
       </c>
@@ -2600,9 +2681,9 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="55"/>
-      <c r="B65" s="72"/>
-      <c r="C65" s="73"/>
+      <c r="A65" s="48"/>
+      <c r="B65" s="59"/>
+      <c r="C65" s="51"/>
       <c r="D65" s="36" t="s">
         <v>133</v>
       </c>
@@ -2615,9 +2696,9 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" s="55"/>
-      <c r="B66" s="72"/>
-      <c r="C66" s="73"/>
+      <c r="A66" s="48"/>
+      <c r="B66" s="59"/>
+      <c r="C66" s="51"/>
       <c r="D66" s="36" t="s">
         <v>134</v>
       </c>
@@ -2630,9 +2711,9 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67" s="55"/>
-      <c r="B67" s="72"/>
-      <c r="C67" s="73" t="s">
+      <c r="A67" s="48"/>
+      <c r="B67" s="59"/>
+      <c r="C67" s="51" t="s">
         <v>142</v>
       </c>
       <c r="D67" s="36" t="s">
@@ -2647,9 +2728,9 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68" s="55"/>
-      <c r="B68" s="72"/>
-      <c r="C68" s="73"/>
+      <c r="A68" s="48"/>
+      <c r="B68" s="59"/>
+      <c r="C68" s="51"/>
       <c r="D68" s="36" t="s">
         <v>129</v>
       </c>
@@ -2662,9 +2743,9 @@
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A69" s="55"/>
-      <c r="B69" s="72"/>
-      <c r="C69" s="73"/>
+      <c r="A69" s="48"/>
+      <c r="B69" s="59"/>
+      <c r="C69" s="51"/>
       <c r="D69" s="36" t="s">
         <v>130</v>
       </c>
@@ -2677,9 +2758,9 @@
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A70" s="55"/>
-      <c r="B70" s="72"/>
-      <c r="C70" s="73"/>
+      <c r="A70" s="48"/>
+      <c r="B70" s="59"/>
+      <c r="C70" s="51"/>
       <c r="D70" s="36" t="s">
         <v>131</v>
       </c>
@@ -2692,9 +2773,9 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A71" s="55"/>
-      <c r="B71" s="72"/>
-      <c r="C71" s="73"/>
+      <c r="A71" s="48"/>
+      <c r="B71" s="59"/>
+      <c r="C71" s="51"/>
       <c r="D71" s="36" t="s">
         <v>132</v>
       </c>
@@ -2707,9 +2788,9 @@
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A72" s="55"/>
-      <c r="B72" s="72"/>
-      <c r="C72" s="73"/>
+      <c r="A72" s="48"/>
+      <c r="B72" s="59"/>
+      <c r="C72" s="51"/>
       <c r="D72" s="36" t="s">
         <v>133</v>
       </c>
@@ -2722,9 +2803,9 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A73" s="55"/>
-      <c r="B73" s="72"/>
-      <c r="C73" s="73"/>
+      <c r="A73" s="48"/>
+      <c r="B73" s="59"/>
+      <c r="C73" s="51"/>
       <c r="D73" s="36" t="s">
         <v>134</v>
       </c>
@@ -2737,9 +2818,9 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" s="55"/>
-      <c r="B74" s="72"/>
-      <c r="C74" s="72" t="s">
+      <c r="A74" s="48"/>
+      <c r="B74" s="59"/>
+      <c r="C74" s="59" t="s">
         <v>150</v>
       </c>
       <c r="D74" s="36" t="s">
@@ -2754,9 +2835,9 @@
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A75" s="55"/>
-      <c r="B75" s="72"/>
-      <c r="C75" s="72"/>
+      <c r="A75" s="48"/>
+      <c r="B75" s="59"/>
+      <c r="C75" s="59"/>
       <c r="D75" s="36" t="s">
         <v>129</v>
       </c>
@@ -2769,9 +2850,9 @@
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A76" s="55"/>
-      <c r="B76" s="72"/>
-      <c r="C76" s="72"/>
+      <c r="A76" s="48"/>
+      <c r="B76" s="59"/>
+      <c r="C76" s="59"/>
       <c r="D76" s="36" t="s">
         <v>130</v>
       </c>
@@ -2784,9 +2865,9 @@
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A77" s="55"/>
-      <c r="B77" s="72"/>
-      <c r="C77" s="72"/>
+      <c r="A77" s="48"/>
+      <c r="B77" s="59"/>
+      <c r="C77" s="59"/>
       <c r="D77" s="36" t="s">
         <v>131</v>
       </c>
@@ -2799,9 +2880,9 @@
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A78" s="55"/>
-      <c r="B78" s="72"/>
-      <c r="C78" s="72"/>
+      <c r="A78" s="48"/>
+      <c r="B78" s="59"/>
+      <c r="C78" s="59"/>
       <c r="D78" s="36" t="s">
         <v>132</v>
       </c>
@@ -2814,9 +2895,9 @@
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A79" s="55"/>
-      <c r="B79" s="72"/>
-      <c r="C79" s="72"/>
+      <c r="A79" s="48"/>
+      <c r="B79" s="59"/>
+      <c r="C79" s="59"/>
       <c r="D79" s="36" t="s">
         <v>133</v>
       </c>
@@ -2829,9 +2910,9 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A80" s="55"/>
-      <c r="B80" s="72"/>
-      <c r="C80" s="72"/>
+      <c r="A80" s="48"/>
+      <c r="B80" s="59"/>
+      <c r="C80" s="59"/>
       <c r="D80" s="36" t="s">
         <v>134</v>
       </c>
@@ -2844,9 +2925,9 @@
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A81" s="55"/>
-      <c r="B81" s="72"/>
-      <c r="C81" s="72" t="s">
+      <c r="A81" s="48"/>
+      <c r="B81" s="59"/>
+      <c r="C81" s="59" t="s">
         <v>182</v>
       </c>
       <c r="D81" s="36" t="s">
@@ -2861,9 +2942,9 @@
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A82" s="55"/>
-      <c r="B82" s="72"/>
-      <c r="C82" s="72"/>
+      <c r="A82" s="48"/>
+      <c r="B82" s="59"/>
+      <c r="C82" s="59"/>
       <c r="D82" s="36" t="s">
         <v>129</v>
       </c>
@@ -2876,9 +2957,9 @@
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A83" s="55"/>
-      <c r="B83" s="72"/>
-      <c r="C83" s="72"/>
+      <c r="A83" s="48"/>
+      <c r="B83" s="59"/>
+      <c r="C83" s="59"/>
       <c r="D83" s="36" t="s">
         <v>130</v>
       </c>
@@ -2891,9 +2972,9 @@
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A84" s="55"/>
-      <c r="B84" s="72"/>
-      <c r="C84" s="72"/>
+      <c r="A84" s="48"/>
+      <c r="B84" s="59"/>
+      <c r="C84" s="59"/>
       <c r="D84" s="36" t="s">
         <v>131</v>
       </c>
@@ -2906,9 +2987,9 @@
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A85" s="55"/>
-      <c r="B85" s="72"/>
-      <c r="C85" s="72"/>
+      <c r="A85" s="48"/>
+      <c r="B85" s="59"/>
+      <c r="C85" s="59"/>
       <c r="D85" s="36" t="s">
         <v>132</v>
       </c>
@@ -2921,9 +3002,9 @@
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A86" s="55"/>
-      <c r="B86" s="72"/>
-      <c r="C86" s="72"/>
+      <c r="A86" s="48"/>
+      <c r="B86" s="59"/>
+      <c r="C86" s="59"/>
       <c r="D86" s="36" t="s">
         <v>133</v>
       </c>
@@ -2936,9 +3017,9 @@
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A87" s="55"/>
-      <c r="B87" s="72"/>
-      <c r="C87" s="72"/>
+      <c r="A87" s="48"/>
+      <c r="B87" s="59"/>
+      <c r="C87" s="59"/>
       <c r="D87" s="36" t="s">
         <v>134</v>
       </c>
@@ -2951,9 +3032,9 @@
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A88" s="55"/>
-      <c r="B88" s="72"/>
-      <c r="C88" s="73" t="s">
+      <c r="A88" s="48"/>
+      <c r="B88" s="59"/>
+      <c r="C88" s="51" t="s">
         <v>181</v>
       </c>
       <c r="D88" s="36" t="s">
@@ -2968,9 +3049,9 @@
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A89" s="55"/>
-      <c r="B89" s="72"/>
-      <c r="C89" s="73"/>
+      <c r="A89" s="48"/>
+      <c r="B89" s="59"/>
+      <c r="C89" s="51"/>
       <c r="D89" s="36" t="s">
         <v>129</v>
       </c>
@@ -2983,9 +3064,9 @@
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A90" s="55"/>
-      <c r="B90" s="72"/>
-      <c r="C90" s="73"/>
+      <c r="A90" s="48"/>
+      <c r="B90" s="59"/>
+      <c r="C90" s="51"/>
       <c r="D90" s="36" t="s">
         <v>130</v>
       </c>
@@ -2998,9 +3079,9 @@
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A91" s="55"/>
-      <c r="B91" s="72"/>
-      <c r="C91" s="73"/>
+      <c r="A91" s="48"/>
+      <c r="B91" s="59"/>
+      <c r="C91" s="51"/>
       <c r="D91" s="36" t="s">
         <v>131</v>
       </c>
@@ -3013,9 +3094,9 @@
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A92" s="55"/>
-      <c r="B92" s="72"/>
-      <c r="C92" s="73"/>
+      <c r="A92" s="48"/>
+      <c r="B92" s="59"/>
+      <c r="C92" s="51"/>
       <c r="D92" s="36" t="s">
         <v>132</v>
       </c>
@@ -3028,9 +3109,9 @@
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A93" s="55"/>
-      <c r="B93" s="72"/>
-      <c r="C93" s="73"/>
+      <c r="A93" s="48"/>
+      <c r="B93" s="59"/>
+      <c r="C93" s="51"/>
       <c r="D93" s="36" t="s">
         <v>133</v>
       </c>
@@ -3043,9 +3124,9 @@
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A94" s="55"/>
-      <c r="B94" s="72"/>
-      <c r="C94" s="73"/>
+      <c r="A94" s="48"/>
+      <c r="B94" s="59"/>
+      <c r="C94" s="51"/>
       <c r="D94" s="36" t="s">
         <v>134</v>
       </c>
@@ -3058,9 +3139,9 @@
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A95" s="55"/>
-      <c r="B95" s="72"/>
-      <c r="C95" s="73" t="s">
+      <c r="A95" s="48"/>
+      <c r="B95" s="59"/>
+      <c r="C95" s="51" t="s">
         <v>172</v>
       </c>
       <c r="D95" s="36" t="s">
@@ -3075,9 +3156,9 @@
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A96" s="55"/>
-      <c r="B96" s="72"/>
-      <c r="C96" s="73"/>
+      <c r="A96" s="48"/>
+      <c r="B96" s="59"/>
+      <c r="C96" s="51"/>
       <c r="D96" s="36" t="s">
         <v>129</v>
       </c>
@@ -3090,9 +3171,9 @@
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A97" s="55"/>
-      <c r="B97" s="72"/>
-      <c r="C97" s="73"/>
+      <c r="A97" s="48"/>
+      <c r="B97" s="59"/>
+      <c r="C97" s="51"/>
       <c r="D97" s="36" t="s">
         <v>130</v>
       </c>
@@ -3105,9 +3186,9 @@
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A98" s="55"/>
-      <c r="B98" s="72"/>
-      <c r="C98" s="73"/>
+      <c r="A98" s="48"/>
+      <c r="B98" s="59"/>
+      <c r="C98" s="51"/>
       <c r="D98" s="36" t="s">
         <v>131</v>
       </c>
@@ -3120,9 +3201,9 @@
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A99" s="55"/>
-      <c r="B99" s="72"/>
-      <c r="C99" s="73"/>
+      <c r="A99" s="48"/>
+      <c r="B99" s="59"/>
+      <c r="C99" s="51"/>
       <c r="D99" s="36" t="s">
         <v>132</v>
       </c>
@@ -3135,9 +3216,9 @@
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A100" s="55"/>
-      <c r="B100" s="72"/>
-      <c r="C100" s="73"/>
+      <c r="A100" s="48"/>
+      <c r="B100" s="59"/>
+      <c r="C100" s="51"/>
       <c r="D100" s="36" t="s">
         <v>133</v>
       </c>
@@ -3150,9 +3231,9 @@
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A101" s="55"/>
-      <c r="B101" s="72"/>
-      <c r="C101" s="73"/>
+      <c r="A101" s="48"/>
+      <c r="B101" s="59"/>
+      <c r="C101" s="51"/>
       <c r="D101" s="36" t="s">
         <v>134</v>
       </c>
@@ -3165,9 +3246,9 @@
       </c>
     </row>
     <row r="102" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="55"/>
-      <c r="B102" s="72"/>
-      <c r="C102" s="72" t="s">
+      <c r="A102" s="48"/>
+      <c r="B102" s="59"/>
+      <c r="C102" s="59" t="s">
         <v>180</v>
       </c>
       <c r="D102" s="36" t="s">
@@ -3182,9 +3263,9 @@
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A103" s="55"/>
-      <c r="B103" s="72"/>
-      <c r="C103" s="72"/>
+      <c r="A103" s="48"/>
+      <c r="B103" s="59"/>
+      <c r="C103" s="59"/>
       <c r="D103" s="36" t="s">
         <v>129</v>
       </c>
@@ -3197,9 +3278,9 @@
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A104" s="55"/>
-      <c r="B104" s="72"/>
-      <c r="C104" s="72"/>
+      <c r="A104" s="48"/>
+      <c r="B104" s="59"/>
+      <c r="C104" s="59"/>
       <c r="D104" s="36" t="s">
         <v>130</v>
       </c>
@@ -3212,9 +3293,9 @@
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A105" s="55"/>
-      <c r="B105" s="72"/>
-      <c r="C105" s="72"/>
+      <c r="A105" s="48"/>
+      <c r="B105" s="59"/>
+      <c r="C105" s="59"/>
       <c r="D105" s="36" t="s">
         <v>131</v>
       </c>
@@ -3227,9 +3308,9 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A106" s="55"/>
-      <c r="B106" s="72"/>
-      <c r="C106" s="72"/>
+      <c r="A106" s="48"/>
+      <c r="B106" s="59"/>
+      <c r="C106" s="59"/>
       <c r="D106" s="36" t="s">
         <v>132</v>
       </c>
@@ -3242,9 +3323,9 @@
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A107" s="55"/>
-      <c r="B107" s="72"/>
-      <c r="C107" s="72"/>
+      <c r="A107" s="48"/>
+      <c r="B107" s="59"/>
+      <c r="C107" s="59"/>
       <c r="D107" s="36" t="s">
         <v>133</v>
       </c>
@@ -3257,9 +3338,9 @@
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A108" s="55"/>
-      <c r="B108" s="72"/>
-      <c r="C108" s="72"/>
+      <c r="A108" s="48"/>
+      <c r="B108" s="59"/>
+      <c r="C108" s="59"/>
       <c r="D108" s="36" t="s">
         <v>134</v>
       </c>
@@ -3272,9 +3353,9 @@
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A109" s="55"/>
-      <c r="B109" s="72"/>
-      <c r="C109" s="73" t="s">
+      <c r="A109" s="48"/>
+      <c r="B109" s="59"/>
+      <c r="C109" s="51" t="s">
         <v>190</v>
       </c>
       <c r="D109" s="36" t="s">
@@ -3289,9 +3370,9 @@
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A110" s="55"/>
-      <c r="B110" s="72"/>
-      <c r="C110" s="73"/>
+      <c r="A110" s="48"/>
+      <c r="B110" s="59"/>
+      <c r="C110" s="51"/>
       <c r="D110" s="36" t="s">
         <v>129</v>
       </c>
@@ -3304,9 +3385,9 @@
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A111" s="55"/>
-      <c r="B111" s="72"/>
-      <c r="C111" s="73"/>
+      <c r="A111" s="48"/>
+      <c r="B111" s="59"/>
+      <c r="C111" s="51"/>
       <c r="D111" s="36" t="s">
         <v>130</v>
       </c>
@@ -3319,9 +3400,9 @@
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A112" s="55"/>
-      <c r="B112" s="72"/>
-      <c r="C112" s="73"/>
+      <c r="A112" s="48"/>
+      <c r="B112" s="59"/>
+      <c r="C112" s="51"/>
       <c r="D112" s="36" t="s">
         <v>131</v>
       </c>
@@ -3334,9 +3415,9 @@
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A113" s="55"/>
-      <c r="B113" s="72"/>
-      <c r="C113" s="73"/>
+      <c r="A113" s="48"/>
+      <c r="B113" s="59"/>
+      <c r="C113" s="51"/>
       <c r="D113" s="36" t="s">
         <v>132</v>
       </c>
@@ -3349,9 +3430,9 @@
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A114" s="55"/>
-      <c r="B114" s="72"/>
-      <c r="C114" s="73"/>
+      <c r="A114" s="48"/>
+      <c r="B114" s="59"/>
+      <c r="C114" s="51"/>
       <c r="D114" s="36" t="s">
         <v>133</v>
       </c>
@@ -3364,9 +3445,9 @@
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A115" s="55"/>
-      <c r="B115" s="72"/>
-      <c r="C115" s="73"/>
+      <c r="A115" s="48"/>
+      <c r="B115" s="59"/>
+      <c r="C115" s="51"/>
       <c r="D115" s="36" t="s">
         <v>134</v>
       </c>
@@ -3379,14 +3460,14 @@
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A116" s="56" t="s">
+      <c r="A116" s="58" t="s">
         <v>198</v>
       </c>
-      <c r="B116" s="71" t="s">
+      <c r="B116" s="49" t="s">
         <v>199</v>
       </c>
-      <c r="C116" s="71"/>
-      <c r="D116" s="71"/>
+      <c r="C116" s="49"/>
+      <c r="D116" s="49"/>
       <c r="E116" s="37"/>
       <c r="F116" s="9" t="s">
         <v>200</v>
@@ -3396,12 +3477,12 @@
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A117" s="56"/>
-      <c r="B117" s="75" t="s">
+      <c r="A117" s="58"/>
+      <c r="B117" s="47" t="s">
         <v>201</v>
       </c>
-      <c r="C117" s="71"/>
-      <c r="D117" s="71"/>
+      <c r="C117" s="49"/>
+      <c r="D117" s="49"/>
       <c r="E117" s="37"/>
       <c r="F117" s="9" t="s">
         <v>202</v>
@@ -3411,12 +3492,12 @@
       </c>
     </row>
     <row r="118" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="56"/>
-      <c r="B118" s="75" t="s">
+      <c r="A118" s="58"/>
+      <c r="B118" s="47" t="s">
         <v>205</v>
       </c>
-      <c r="C118" s="75"/>
-      <c r="D118" s="75"/>
+      <c r="C118" s="47"/>
+      <c r="D118" s="47"/>
       <c r="E118" s="38"/>
       <c r="F118" s="9" t="s">
         <v>206</v>
@@ -3426,12 +3507,12 @@
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A119" s="56"/>
-      <c r="B119" s="71" t="s">
+      <c r="A119" s="58"/>
+      <c r="B119" s="49" t="s">
         <v>203</v>
       </c>
-      <c r="C119" s="71"/>
-      <c r="D119" s="71"/>
+      <c r="C119" s="49"/>
+      <c r="D119" s="49"/>
       <c r="E119" s="37"/>
       <c r="F119" s="9" t="s">
         <v>204</v>
@@ -3448,6 +3529,49 @@
     </row>
   </sheetData>
   <mergeCells count="59">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="A25:A37"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A14"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="A38:A43"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="B20:C24"/>
+    <mergeCell ref="B25:C29"/>
+    <mergeCell ref="B30:C34"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B50:C57"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B41:C43"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="E46:E49"/>
+    <mergeCell ref="B119:D119"/>
+    <mergeCell ref="A116:A119"/>
+    <mergeCell ref="C74:C80"/>
+    <mergeCell ref="C81:C87"/>
+    <mergeCell ref="C88:C94"/>
+    <mergeCell ref="C95:C101"/>
+    <mergeCell ref="C102:C108"/>
+    <mergeCell ref="C109:C115"/>
+    <mergeCell ref="B60:B115"/>
+    <mergeCell ref="A46:A57"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B118:D118"/>
     <mergeCell ref="A58:A115"/>
@@ -3464,49 +3588,6 @@
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E46:E49"/>
-    <mergeCell ref="B119:D119"/>
-    <mergeCell ref="A116:A119"/>
-    <mergeCell ref="C74:C80"/>
-    <mergeCell ref="C81:C87"/>
-    <mergeCell ref="C88:C94"/>
-    <mergeCell ref="C95:C101"/>
-    <mergeCell ref="C102:C108"/>
-    <mergeCell ref="C109:C115"/>
-    <mergeCell ref="B60:B115"/>
-    <mergeCell ref="A46:A57"/>
-    <mergeCell ref="B25:C29"/>
-    <mergeCell ref="B30:C34"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B50:C57"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B41:C43"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="B20:C24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="A25:A37"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A14"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="A38:A43"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3517,7 +3598,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3529,12 +3610,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="80" t="s">
         <v>223</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
       <c r="E1" s="39"/>
       <c r="F1" s="39"/>
     </row>
@@ -3552,29 +3633,29 @@
         <v>208</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="s">
         <v>226</v>
       </c>
       <c r="B4" s="42" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="D4" s="32" t="s">
         <v>214</v>
@@ -3596,7 +3677,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="41" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B6" s="32" t="s">
         <v>230</v>
@@ -3617,7 +3698,7 @@
       </c>
       <c r="C7" s="32"/>
       <c r="D7" s="32" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -3631,7 +3712,7 @@
         <v>237</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -3645,19 +3726,19 @@
         <v>238</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="41" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B10" s="32" t="s">
         <v>239</v>
       </c>
       <c r="C10" s="32"/>
       <c r="D10" s="32" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -3668,7 +3749,7 @@
         <v>241</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>242</v>
+        <v>259</v>
       </c>
       <c r="D11" s="32" t="s">
         <v>214</v>
@@ -3676,30 +3757,192 @@
     </row>
     <row r="12" spans="1:6" ht="192" x14ac:dyDescent="0.2">
       <c r="A12" s="41" t="s">
+        <v>242</v>
+      </c>
+      <c r="B12" s="32" t="s">
         <v>243</v>
       </c>
-      <c r="B12" s="32" t="s">
-        <v>244</v>
-      </c>
       <c r="C12" s="42" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="41" t="s">
+        <v>244</v>
+      </c>
+      <c r="B13" s="32" t="s">
         <v>245</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="C13" s="32" t="s">
         <v>246</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="D13" s="32" t="s">
+        <v>253</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="36.83203125" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
+    <col min="4" max="4" width="47.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1" s="81" t="s">
+        <v>260</v>
+      </c>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="44" t="s">
+        <v>225</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>224</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>207</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>261</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="42" t="s">
         <v>247</v>
       </c>
-      <c r="D13" s="32" t="s">
-        <v>255</v>
+      <c r="C4" s="42" t="s">
+        <v>257</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" s="45" t="s">
+        <v>263</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>268</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>273</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="45" t="s">
+        <v>265</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>269</v>
+      </c>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="45" t="s">
+        <v>267</v>
+      </c>
+      <c r="B7" s="42" t="s">
+        <v>270</v>
+      </c>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="45" t="s">
+        <v>280</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>281</v>
+      </c>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" s="45" t="s">
+        <v>272</v>
+      </c>
+      <c r="B9" s="42" t="s">
+        <v>274</v>
+      </c>
+      <c r="C9" s="42" t="s">
+        <v>273</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="45" t="s">
+        <v>278</v>
+      </c>
+      <c r="B10" s="42" t="s">
+        <v>279</v>
+      </c>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="45" t="s">
+        <v>275</v>
+      </c>
+      <c r="B11" s="42" t="s">
+        <v>276</v>
+      </c>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added final question in the survey mobility
</commit_message>
<xml_diff>
--- a/data_dict.xlsx
+++ b/data_dict.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="tabla-survey" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="288">
   <si>
     <t>Pregunta</t>
   </si>
@@ -924,6 +924,12 @@
   </si>
   <si>
     <t>Esta en m/s</t>
+  </si>
+  <si>
+    <t>tarot_movilidad</t>
+  </si>
+  <si>
+    <t>Para usted, ¿Cuál de estas imágenes representa su movilidad, y por qué?.</t>
   </si>
 </sst>
 </file>
@@ -1215,10 +1221,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1271,12 +1276,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1294,114 +1293,122 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1681,8 +1688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G120"/>
   <sheetViews>
-    <sheetView topLeftCell="C37" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1697,213 +1704,213 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="45" t="s">
         <v>221</v>
       </c>
-      <c r="B1" s="68"/>
+      <c r="B1" s="45"/>
     </row>
     <row r="2" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="24" t="s">
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="25" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4" t="s">
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="26" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="60"/>
-      <c r="B4" s="79" t="s">
+      <c r="A4" s="56"/>
+      <c r="B4" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="43" t="s">
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="40" t="s">
         <v>257</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="26" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="7" t="s">
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="27" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="48"/>
-      <c r="B6" s="50" t="s">
+      <c r="A6" s="57"/>
+      <c r="B6" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7" t="s">
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="28" t="s">
+      <c r="G6" s="27" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="48"/>
-      <c r="B7" s="50" t="s">
+      <c r="A7" s="57"/>
+      <c r="B7" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7" t="s">
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="28" t="s">
+      <c r="G7" s="27" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="48"/>
-      <c r="B8" s="50" t="s">
+      <c r="A8" s="57"/>
+      <c r="B8" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="7" t="s">
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="27" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="48"/>
-      <c r="B9" s="50" t="s">
+      <c r="A9" s="57"/>
+      <c r="B9" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="7" t="s">
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="48"/>
-      <c r="B10" s="50" t="s">
+      <c r="A10" s="57"/>
+      <c r="B10" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="7" t="s">
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="27" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="48"/>
-      <c r="B11" s="50" t="s">
+      <c r="A11" s="57"/>
+      <c r="B11" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="7" t="s">
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="27" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="48"/>
-      <c r="B12" s="50" t="s">
+      <c r="A12" s="57"/>
+      <c r="B12" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="7" t="s">
+      <c r="C12" s="55"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="28" t="s">
+      <c r="G12" s="27" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="48"/>
-      <c r="B13" s="50" t="s">
+      <c r="A13" s="57"/>
+      <c r="B13" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="7" t="s">
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="28" t="s">
+      <c r="G13" s="27" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="48"/>
-      <c r="B14" s="50" t="s">
+      <c r="A14" s="57"/>
+      <c r="B14" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="7" t="s">
+      <c r="C14" s="55"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="28" t="s">
+      <c r="G14" s="27" t="s">
         <v>212</v>
       </c>
     </row>
@@ -1911,1560 +1918,1560 @@
       <c r="A15" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="54" t="s">
+      <c r="B15" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="9" t="s">
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="29" t="s">
+      <c r="G15" s="28" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="58"/>
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="54"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="9" t="s">
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="G16" s="29" t="s">
+      <c r="G16" s="28" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="58"/>
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="9" t="s">
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="29" t="s">
+      <c r="G17" s="28" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="58"/>
-      <c r="B18" s="54" t="s">
+      <c r="B18" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="9" t="s">
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="G18" s="29" t="s">
+      <c r="G18" s="28" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="58"/>
-      <c r="B19" s="54" t="s">
+      <c r="B19" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="9" t="s">
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G19" s="29" t="s">
+      <c r="G19" s="28" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="66" t="s">
+      <c r="A20" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="67" t="s">
+      <c r="B20" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="67"/>
-      <c r="D20" s="10" t="s">
+      <c r="C20" s="63"/>
+      <c r="D20" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="10"/>
-      <c r="F20" s="12" t="s">
+      <c r="E20" s="9"/>
+      <c r="F20" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="G20" s="30" t="s">
+      <c r="G20" s="29" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="66"/>
-      <c r="B21" s="67"/>
-      <c r="C21" s="67"/>
-      <c r="D21" s="11" t="s">
+      <c r="A21" s="62"/>
+      <c r="B21" s="63"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="12" t="s">
+      <c r="E21" s="10"/>
+      <c r="F21" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G21" s="30" t="s">
+      <c r="G21" s="29" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="66"/>
-      <c r="B22" s="67"/>
-      <c r="C22" s="67"/>
-      <c r="D22" s="11" t="s">
+      <c r="A22" s="62"/>
+      <c r="B22" s="63"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="12" t="s">
+      <c r="E22" s="10"/>
+      <c r="F22" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G22" s="30" t="s">
+      <c r="G22" s="29" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="66"/>
-      <c r="B23" s="67"/>
-      <c r="C23" s="67"/>
-      <c r="D23" s="11" t="s">
+      <c r="A23" s="62"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="63"/>
+      <c r="D23" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="12" t="s">
+      <c r="E23" s="10"/>
+      <c r="F23" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="G23" s="30" t="s">
+      <c r="G23" s="29" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="66"/>
-      <c r="B24" s="67"/>
-      <c r="C24" s="67"/>
-      <c r="D24" s="11" t="s">
+      <c r="A24" s="62"/>
+      <c r="B24" s="63"/>
+      <c r="C24" s="63"/>
+      <c r="D24" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="12" t="s">
+      <c r="E24" s="10"/>
+      <c r="F24" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="G24" s="30" t="s">
+      <c r="G24" s="29" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="75" t="s">
+      <c r="A25" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="61" t="s">
+      <c r="B25" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="61"/>
-      <c r="D25" s="13" t="s">
+      <c r="C25" s="64"/>
+      <c r="D25" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E25" s="13"/>
-      <c r="F25" s="14" t="s">
+      <c r="E25" s="12"/>
+      <c r="F25" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="G25" s="31" t="s">
+      <c r="G25" s="30" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="76"/>
-      <c r="B26" s="61"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="13" t="s">
+      <c r="A26" s="53"/>
+      <c r="B26" s="64"/>
+      <c r="C26" s="64"/>
+      <c r="D26" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="14" t="s">
+      <c r="E26" s="12"/>
+      <c r="F26" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="G26" s="31" t="s">
+      <c r="G26" s="30" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="76"/>
-      <c r="B27" s="61"/>
-      <c r="C27" s="61"/>
-      <c r="D27" s="13" t="s">
+      <c r="A27" s="53"/>
+      <c r="B27" s="64"/>
+      <c r="C27" s="64"/>
+      <c r="D27" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E27" s="13"/>
-      <c r="F27" s="14" t="s">
+      <c r="E27" s="12"/>
+      <c r="F27" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G27" s="31" t="s">
+      <c r="G27" s="30" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="76"/>
-      <c r="B28" s="61"/>
-      <c r="C28" s="61"/>
-      <c r="D28" s="13" t="s">
+      <c r="A28" s="53"/>
+      <c r="B28" s="64"/>
+      <c r="C28" s="64"/>
+      <c r="D28" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="E28" s="13"/>
-      <c r="F28" s="14" t="s">
+      <c r="E28" s="12"/>
+      <c r="F28" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="G28" s="31" t="s">
+      <c r="G28" s="30" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="76"/>
-      <c r="B29" s="61"/>
-      <c r="C29" s="61"/>
-      <c r="D29" s="13" t="s">
+      <c r="A29" s="53"/>
+      <c r="B29" s="64"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="13"/>
-      <c r="F29" s="14" t="s">
+      <c r="E29" s="12"/>
+      <c r="F29" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="G29" s="31" t="s">
+      <c r="G29" s="30" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="76"/>
-      <c r="B30" s="61" t="s">
+      <c r="A30" s="53"/>
+      <c r="B30" s="64" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="61"/>
-      <c r="D30" s="13" t="s">
+      <c r="C30" s="64"/>
+      <c r="D30" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E30" s="13"/>
-      <c r="F30" s="14" t="s">
+      <c r="E30" s="12"/>
+      <c r="F30" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="G30" s="31" t="s">
+      <c r="G30" s="30" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="76"/>
-      <c r="B31" s="61"/>
-      <c r="C31" s="61"/>
-      <c r="D31" s="13" t="s">
+      <c r="A31" s="53"/>
+      <c r="B31" s="64"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E31" s="13"/>
-      <c r="F31" s="14" t="s">
+      <c r="E31" s="12"/>
+      <c r="F31" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="G31" s="31" t="s">
+      <c r="G31" s="30" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="76"/>
-      <c r="B32" s="61"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="13" t="s">
+      <c r="A32" s="53"/>
+      <c r="B32" s="64"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="E32" s="13"/>
-      <c r="F32" s="14" t="s">
+      <c r="E32" s="12"/>
+      <c r="F32" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="G32" s="31" t="s">
+      <c r="G32" s="30" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="76"/>
-      <c r="B33" s="61"/>
-      <c r="C33" s="61"/>
-      <c r="D33" s="13" t="s">
+      <c r="A33" s="53"/>
+      <c r="B33" s="64"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E33" s="13"/>
-      <c r="F33" s="14" t="s">
+      <c r="E33" s="12"/>
+      <c r="F33" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="G33" s="31" t="s">
+      <c r="G33" s="30" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="76"/>
-      <c r="B34" s="61"/>
-      <c r="C34" s="61"/>
-      <c r="D34" s="13" t="s">
+      <c r="A34" s="53"/>
+      <c r="B34" s="64"/>
+      <c r="C34" s="64"/>
+      <c r="D34" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="E34" s="13"/>
-      <c r="F34" s="14" t="s">
+      <c r="E34" s="12"/>
+      <c r="F34" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="G34" s="31" t="s">
+      <c r="G34" s="30" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="76"/>
-      <c r="B35" s="72" t="s">
+      <c r="A35" s="53"/>
+      <c r="B35" s="49" t="s">
         <v>215</v>
       </c>
-      <c r="C35" s="73"/>
-      <c r="D35" s="74"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="14" t="s">
+      <c r="C35" s="50"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="G35" s="31" t="s">
+      <c r="G35" s="30" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="76"/>
-      <c r="B36" s="72" t="s">
+      <c r="A36" s="53"/>
+      <c r="B36" s="49" t="s">
         <v>217</v>
       </c>
-      <c r="C36" s="73"/>
-      <c r="D36" s="74"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="14" t="s">
+      <c r="C36" s="50"/>
+      <c r="D36" s="51"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="G36" s="31" t="s">
+      <c r="G36" s="30" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="77"/>
-      <c r="B37" s="72" t="s">
+      <c r="A37" s="54"/>
+      <c r="B37" s="49" t="s">
         <v>219</v>
       </c>
-      <c r="C37" s="73"/>
-      <c r="D37" s="74"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="14" t="s">
+      <c r="C37" s="50"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="G37" s="31" t="s">
+      <c r="G37" s="30" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="78" t="s">
+      <c r="A38" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="B38" s="69" t="s">
+      <c r="B38" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="70"/>
-      <c r="D38" s="71"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="18" t="s">
+      <c r="C38" s="47"/>
+      <c r="D38" s="48"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="G38" s="32" t="s">
+      <c r="G38" s="31" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="78"/>
-      <c r="B39" s="62" t="s">
+      <c r="A39" s="60"/>
+      <c r="B39" s="66" t="s">
         <v>78</v>
       </c>
-      <c r="C39" s="62"/>
-      <c r="D39" s="62"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="18" t="s">
+      <c r="C39" s="66"/>
+      <c r="D39" s="66"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="G39" s="32" t="s">
+      <c r="G39" s="31" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="78"/>
-      <c r="B40" s="62" t="s">
+      <c r="A40" s="60"/>
+      <c r="B40" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="C40" s="62"/>
-      <c r="D40" s="62"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="18" t="s">
+      <c r="C40" s="66"/>
+      <c r="D40" s="66"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="G40" s="32" t="s">
+      <c r="G40" s="31" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="78"/>
-      <c r="B41" s="63" t="s">
+      <c r="A41" s="60"/>
+      <c r="B41" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="C41" s="63"/>
-      <c r="D41" s="17" t="s">
+      <c r="C41" s="67"/>
+      <c r="D41" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E41" s="17"/>
-      <c r="F41" s="18" t="s">
+      <c r="E41" s="16"/>
+      <c r="F41" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="G41" s="32" t="s">
+      <c r="G41" s="31" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="78"/>
-      <c r="B42" s="63"/>
-      <c r="C42" s="63"/>
-      <c r="D42" s="17" t="s">
+      <c r="A42" s="60"/>
+      <c r="B42" s="67"/>
+      <c r="C42" s="67"/>
+      <c r="D42" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="E42" s="17"/>
-      <c r="F42" s="18" t="s">
+      <c r="E42" s="16"/>
+      <c r="F42" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="G42" s="32" t="s">
+      <c r="G42" s="31" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="78"/>
-      <c r="B43" s="63"/>
-      <c r="C43" s="63"/>
-      <c r="D43" s="17" t="s">
+      <c r="A43" s="60"/>
+      <c r="B43" s="67"/>
+      <c r="C43" s="67"/>
+      <c r="D43" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="E43" s="17"/>
-      <c r="F43" s="18" t="s">
+      <c r="E43" s="16"/>
+      <c r="F43" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="G43" s="32" t="s">
+      <c r="G43" s="31" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="52" t="s">
+      <c r="A44" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="B44" s="65" t="s">
+      <c r="B44" s="69" t="s">
         <v>89</v>
       </c>
-      <c r="C44" s="65"/>
-      <c r="D44" s="65"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="21" t="s">
+      <c r="C44" s="69"/>
+      <c r="D44" s="69"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="G44" s="33" t="s">
+      <c r="G44" s="32" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="52"/>
-      <c r="B45" s="64" t="s">
+      <c r="A45" s="78"/>
+      <c r="B45" s="68" t="s">
         <v>91</v>
       </c>
-      <c r="C45" s="64"/>
-      <c r="D45" s="64"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="21" t="s">
+      <c r="C45" s="68"/>
+      <c r="D45" s="68"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="G45" s="33" t="s">
+      <c r="G45" s="32" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="60" t="s">
+      <c r="A46" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="B46" s="53" t="s">
+      <c r="B46" s="65" t="s">
         <v>94</v>
       </c>
-      <c r="C46" s="53"/>
-      <c r="D46" s="22" t="s">
+      <c r="C46" s="65"/>
+      <c r="D46" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="E46" s="55" t="s">
+      <c r="E46" s="70" t="s">
         <v>103</v>
       </c>
-      <c r="F46" s="5" t="s">
+      <c r="F46" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="G46" s="34" t="s">
+      <c r="G46" s="33" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="60"/>
-      <c r="B47" s="53"/>
-      <c r="C47" s="53"/>
-      <c r="D47" s="22" t="s">
+      <c r="A47" s="56"/>
+      <c r="B47" s="65"/>
+      <c r="C47" s="65"/>
+      <c r="D47" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="E47" s="56"/>
-      <c r="F47" s="5" t="s">
+      <c r="E47" s="71"/>
+      <c r="F47" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="G47" s="34" t="s">
+      <c r="G47" s="33" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="60"/>
-      <c r="B48" s="53"/>
-      <c r="C48" s="53"/>
-      <c r="D48" s="22" t="s">
+      <c r="A48" s="56"/>
+      <c r="B48" s="65"/>
+      <c r="C48" s="65"/>
+      <c r="D48" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="E48" s="56"/>
-      <c r="F48" s="5" t="s">
+      <c r="E48" s="71"/>
+      <c r="F48" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="G48" s="34" t="s">
+      <c r="G48" s="33" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="60"/>
-      <c r="B49" s="53"/>
-      <c r="C49" s="53"/>
-      <c r="D49" s="22" t="s">
+      <c r="A49" s="56"/>
+      <c r="B49" s="65"/>
+      <c r="C49" s="65"/>
+      <c r="D49" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="E49" s="57"/>
-      <c r="F49" s="5" t="s">
+      <c r="E49" s="72"/>
+      <c r="F49" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="G49" s="34" t="s">
+      <c r="G49" s="33" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="60"/>
-      <c r="B50" s="53" t="s">
+      <c r="A50" s="56"/>
+      <c r="B50" s="65" t="s">
         <v>104</v>
       </c>
-      <c r="C50" s="53"/>
-      <c r="D50" s="22" t="s">
+      <c r="C50" s="65"/>
+      <c r="D50" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="E50" s="22"/>
-      <c r="F50" s="5" t="s">
+      <c r="E50" s="21"/>
+      <c r="F50" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="G50" s="34" t="s">
+      <c r="G50" s="33" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="60"/>
-      <c r="B51" s="53"/>
-      <c r="C51" s="53"/>
-      <c r="D51" s="22" t="s">
+      <c r="A51" s="56"/>
+      <c r="B51" s="65"/>
+      <c r="C51" s="65"/>
+      <c r="D51" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="E51" s="22"/>
-      <c r="F51" s="5" t="s">
+      <c r="E51" s="21"/>
+      <c r="F51" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="G51" s="34" t="s">
+      <c r="G51" s="33" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="60"/>
-      <c r="B52" s="53"/>
-      <c r="C52" s="53"/>
-      <c r="D52" s="22" t="s">
+      <c r="A52" s="56"/>
+      <c r="B52" s="65"/>
+      <c r="C52" s="65"/>
+      <c r="D52" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="E52" s="22"/>
-      <c r="F52" s="5" t="s">
+      <c r="E52" s="21"/>
+      <c r="F52" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="G52" s="34" t="s">
+      <c r="G52" s="33" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="60"/>
-      <c r="B53" s="53"/>
-      <c r="C53" s="53"/>
-      <c r="D53" s="22" t="s">
+      <c r="A53" s="56"/>
+      <c r="B53" s="65"/>
+      <c r="C53" s="65"/>
+      <c r="D53" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="E53" s="22"/>
-      <c r="F53" s="5" t="s">
+      <c r="E53" s="21"/>
+      <c r="F53" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="G53" s="34" t="s">
+      <c r="G53" s="33" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" s="60"/>
-      <c r="B54" s="53"/>
-      <c r="C54" s="53"/>
-      <c r="D54" s="22" t="s">
+      <c r="A54" s="56"/>
+      <c r="B54" s="65"/>
+      <c r="C54" s="65"/>
+      <c r="D54" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="E54" s="22"/>
-      <c r="F54" s="5" t="s">
+      <c r="E54" s="21"/>
+      <c r="F54" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="G54" s="34" t="s">
+      <c r="G54" s="33" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="60"/>
-      <c r="B55" s="53"/>
-      <c r="C55" s="53"/>
-      <c r="D55" s="22" t="s">
+      <c r="A55" s="56"/>
+      <c r="B55" s="65"/>
+      <c r="C55" s="65"/>
+      <c r="D55" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="E55" s="22"/>
-      <c r="F55" s="5" t="s">
+      <c r="E55" s="21"/>
+      <c r="F55" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="G55" s="34" t="s">
+      <c r="G55" s="33" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="60"/>
-      <c r="B56" s="53"/>
-      <c r="C56" s="53"/>
-      <c r="D56" s="22" t="s">
+      <c r="A56" s="56"/>
+      <c r="B56" s="65"/>
+      <c r="C56" s="65"/>
+      <c r="D56" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="E56" s="22"/>
-      <c r="F56" s="5" t="s">
+      <c r="E56" s="21"/>
+      <c r="F56" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="G56" s="34" t="s">
+      <c r="G56" s="33" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="60"/>
-      <c r="B57" s="53"/>
-      <c r="C57" s="53"/>
-      <c r="D57" s="22" t="s">
+      <c r="A57" s="56"/>
+      <c r="B57" s="65"/>
+      <c r="C57" s="65"/>
+      <c r="D57" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="E57" s="22"/>
-      <c r="F57" s="5" t="s">
+      <c r="E57" s="21"/>
+      <c r="F57" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="G57" s="34" t="s">
+      <c r="G57" s="33" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="48" t="s">
+      <c r="A58" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="B58" s="50" t="s">
+      <c r="B58" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="C58" s="50"/>
-      <c r="D58" s="50"/>
-      <c r="E58" s="6"/>
-      <c r="F58" s="35" t="s">
+      <c r="C58" s="55"/>
+      <c r="D58" s="55"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="G58" s="28" t="s">
+      <c r="G58" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="48"/>
-      <c r="B59" s="50" t="s">
+      <c r="A59" s="57"/>
+      <c r="B59" s="55" t="s">
         <v>125</v>
       </c>
-      <c r="C59" s="50"/>
-      <c r="D59" s="50"/>
-      <c r="E59" s="6"/>
-      <c r="F59" s="35" t="s">
+      <c r="C59" s="55"/>
+      <c r="D59" s="55"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="G59" s="28" t="s">
+      <c r="G59" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="48"/>
-      <c r="B60" s="59" t="s">
+      <c r="A60" s="57"/>
+      <c r="B60" s="74" t="s">
         <v>126</v>
       </c>
-      <c r="C60" s="51" t="s">
+      <c r="C60" s="75" t="s">
         <v>127</v>
       </c>
-      <c r="D60" s="36" t="s">
+      <c r="D60" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="E60" s="36"/>
-      <c r="F60" s="35" t="s">
+      <c r="E60" s="35"/>
+      <c r="F60" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="G60" s="28" t="s">
+      <c r="G60" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" s="48"/>
-      <c r="B61" s="59"/>
-      <c r="C61" s="51"/>
-      <c r="D61" s="36" t="s">
+      <c r="A61" s="57"/>
+      <c r="B61" s="74"/>
+      <c r="C61" s="75"/>
+      <c r="D61" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="E61" s="36"/>
-      <c r="F61" s="35" t="s">
+      <c r="E61" s="35"/>
+      <c r="F61" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="G61" s="28" t="s">
+      <c r="G61" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" s="48"/>
-      <c r="B62" s="59"/>
-      <c r="C62" s="51"/>
-      <c r="D62" s="36" t="s">
+      <c r="A62" s="57"/>
+      <c r="B62" s="74"/>
+      <c r="C62" s="75"/>
+      <c r="D62" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="E62" s="36"/>
-      <c r="F62" s="35" t="s">
+      <c r="E62" s="35"/>
+      <c r="F62" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="G62" s="28" t="s">
+      <c r="G62" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="48"/>
-      <c r="B63" s="59"/>
-      <c r="C63" s="51"/>
-      <c r="D63" s="36" t="s">
+      <c r="A63" s="57"/>
+      <c r="B63" s="74"/>
+      <c r="C63" s="75"/>
+      <c r="D63" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="E63" s="36"/>
-      <c r="F63" s="35" t="s">
+      <c r="E63" s="35"/>
+      <c r="F63" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="G63" s="28" t="s">
+      <c r="G63" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" s="48"/>
-      <c r="B64" s="59"/>
-      <c r="C64" s="51"/>
-      <c r="D64" s="36" t="s">
+      <c r="A64" s="57"/>
+      <c r="B64" s="74"/>
+      <c r="C64" s="75"/>
+      <c r="D64" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="E64" s="36"/>
-      <c r="F64" s="35" t="s">
+      <c r="E64" s="35"/>
+      <c r="F64" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="G64" s="28" t="s">
+      <c r="G64" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="48"/>
-      <c r="B65" s="59"/>
-      <c r="C65" s="51"/>
-      <c r="D65" s="36" t="s">
+      <c r="A65" s="57"/>
+      <c r="B65" s="74"/>
+      <c r="C65" s="75"/>
+      <c r="D65" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="E65" s="36"/>
-      <c r="F65" s="35" t="s">
+      <c r="E65" s="35"/>
+      <c r="F65" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="G65" s="28" t="s">
+      <c r="G65" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" s="48"/>
-      <c r="B66" s="59"/>
-      <c r="C66" s="51"/>
-      <c r="D66" s="36" t="s">
+      <c r="A66" s="57"/>
+      <c r="B66" s="74"/>
+      <c r="C66" s="75"/>
+      <c r="D66" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="E66" s="36"/>
-      <c r="F66" s="35" t="s">
+      <c r="E66" s="35"/>
+      <c r="F66" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="G66" s="28" t="s">
+      <c r="G66" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67" s="48"/>
-      <c r="B67" s="59"/>
-      <c r="C67" s="51" t="s">
+      <c r="A67" s="57"/>
+      <c r="B67" s="74"/>
+      <c r="C67" s="75" t="s">
         <v>142</v>
       </c>
-      <c r="D67" s="36" t="s">
+      <c r="D67" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="E67" s="36"/>
-      <c r="F67" s="35" t="s">
+      <c r="E67" s="35"/>
+      <c r="F67" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="G67" s="28" t="s">
+      <c r="G67" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68" s="48"/>
-      <c r="B68" s="59"/>
-      <c r="C68" s="51"/>
-      <c r="D68" s="36" t="s">
+      <c r="A68" s="57"/>
+      <c r="B68" s="74"/>
+      <c r="C68" s="75"/>
+      <c r="D68" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="E68" s="36"/>
-      <c r="F68" s="35" t="s">
+      <c r="E68" s="35"/>
+      <c r="F68" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="G68" s="28" t="s">
+      <c r="G68" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A69" s="48"/>
-      <c r="B69" s="59"/>
-      <c r="C69" s="51"/>
-      <c r="D69" s="36" t="s">
+      <c r="A69" s="57"/>
+      <c r="B69" s="74"/>
+      <c r="C69" s="75"/>
+      <c r="D69" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="E69" s="36"/>
-      <c r="F69" s="35" t="s">
+      <c r="E69" s="35"/>
+      <c r="F69" s="34" t="s">
         <v>145</v>
       </c>
-      <c r="G69" s="28" t="s">
+      <c r="G69" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A70" s="48"/>
-      <c r="B70" s="59"/>
-      <c r="C70" s="51"/>
-      <c r="D70" s="36" t="s">
+      <c r="A70" s="57"/>
+      <c r="B70" s="74"/>
+      <c r="C70" s="75"/>
+      <c r="D70" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="E70" s="36"/>
-      <c r="F70" s="35" t="s">
+      <c r="E70" s="35"/>
+      <c r="F70" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="G70" s="28" t="s">
+      <c r="G70" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A71" s="48"/>
-      <c r="B71" s="59"/>
-      <c r="C71" s="51"/>
-      <c r="D71" s="36" t="s">
+      <c r="A71" s="57"/>
+      <c r="B71" s="74"/>
+      <c r="C71" s="75"/>
+      <c r="D71" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="E71" s="36"/>
-      <c r="F71" s="35" t="s">
+      <c r="E71" s="35"/>
+      <c r="F71" s="34" t="s">
         <v>147</v>
       </c>
-      <c r="G71" s="28" t="s">
+      <c r="G71" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A72" s="48"/>
-      <c r="B72" s="59"/>
-      <c r="C72" s="51"/>
-      <c r="D72" s="36" t="s">
+      <c r="A72" s="57"/>
+      <c r="B72" s="74"/>
+      <c r="C72" s="75"/>
+      <c r="D72" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="E72" s="36"/>
-      <c r="F72" s="35" t="s">
+      <c r="E72" s="35"/>
+      <c r="F72" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="G72" s="28" t="s">
+      <c r="G72" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A73" s="48"/>
-      <c r="B73" s="59"/>
-      <c r="C73" s="51"/>
-      <c r="D73" s="36" t="s">
+      <c r="A73" s="57"/>
+      <c r="B73" s="74"/>
+      <c r="C73" s="75"/>
+      <c r="D73" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="E73" s="36"/>
-      <c r="F73" s="35" t="s">
+      <c r="E73" s="35"/>
+      <c r="F73" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="G73" s="28" t="s">
+      <c r="G73" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" s="48"/>
-      <c r="B74" s="59"/>
-      <c r="C74" s="59" t="s">
+      <c r="A74" s="57"/>
+      <c r="B74" s="74"/>
+      <c r="C74" s="74" t="s">
         <v>150</v>
       </c>
-      <c r="D74" s="36" t="s">
+      <c r="D74" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="E74" s="36"/>
-      <c r="F74" s="35" t="s">
+      <c r="E74" s="35"/>
+      <c r="F74" s="34" t="s">
         <v>151</v>
       </c>
-      <c r="G74" s="28" t="s">
+      <c r="G74" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A75" s="48"/>
-      <c r="B75" s="59"/>
-      <c r="C75" s="59"/>
-      <c r="D75" s="36" t="s">
+      <c r="A75" s="57"/>
+      <c r="B75" s="74"/>
+      <c r="C75" s="74"/>
+      <c r="D75" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="E75" s="36"/>
-      <c r="F75" s="35" t="s">
+      <c r="E75" s="35"/>
+      <c r="F75" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="G75" s="28" t="s">
+      <c r="G75" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A76" s="48"/>
-      <c r="B76" s="59"/>
-      <c r="C76" s="59"/>
-      <c r="D76" s="36" t="s">
+      <c r="A76" s="57"/>
+      <c r="B76" s="74"/>
+      <c r="C76" s="74"/>
+      <c r="D76" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="E76" s="36"/>
-      <c r="F76" s="35" t="s">
+      <c r="E76" s="35"/>
+      <c r="F76" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="G76" s="28" t="s">
+      <c r="G76" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A77" s="48"/>
-      <c r="B77" s="59"/>
-      <c r="C77" s="59"/>
-      <c r="D77" s="36" t="s">
+      <c r="A77" s="57"/>
+      <c r="B77" s="74"/>
+      <c r="C77" s="74"/>
+      <c r="D77" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="E77" s="36"/>
-      <c r="F77" s="35" t="s">
+      <c r="E77" s="35"/>
+      <c r="F77" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="G77" s="28" t="s">
+      <c r="G77" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A78" s="48"/>
-      <c r="B78" s="59"/>
-      <c r="C78" s="59"/>
-      <c r="D78" s="36" t="s">
+      <c r="A78" s="57"/>
+      <c r="B78" s="74"/>
+      <c r="C78" s="74"/>
+      <c r="D78" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="E78" s="36"/>
-      <c r="F78" s="35" t="s">
+      <c r="E78" s="35"/>
+      <c r="F78" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="G78" s="28" t="s">
+      <c r="G78" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A79" s="48"/>
-      <c r="B79" s="59"/>
-      <c r="C79" s="59"/>
-      <c r="D79" s="36" t="s">
+      <c r="A79" s="57"/>
+      <c r="B79" s="74"/>
+      <c r="C79" s="74"/>
+      <c r="D79" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="E79" s="36"/>
-      <c r="F79" s="35" t="s">
+      <c r="E79" s="35"/>
+      <c r="F79" s="34" t="s">
         <v>156</v>
       </c>
-      <c r="G79" s="28" t="s">
+      <c r="G79" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A80" s="48"/>
-      <c r="B80" s="59"/>
-      <c r="C80" s="59"/>
-      <c r="D80" s="36" t="s">
+      <c r="A80" s="57"/>
+      <c r="B80" s="74"/>
+      <c r="C80" s="74"/>
+      <c r="D80" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="E80" s="36"/>
-      <c r="F80" s="35" t="s">
+      <c r="E80" s="35"/>
+      <c r="F80" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="G80" s="28" t="s">
+      <c r="G80" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A81" s="48"/>
-      <c r="B81" s="59"/>
-      <c r="C81" s="59" t="s">
+      <c r="A81" s="57"/>
+      <c r="B81" s="74"/>
+      <c r="C81" s="74" t="s">
         <v>182</v>
       </c>
-      <c r="D81" s="36" t="s">
+      <c r="D81" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="E81" s="36"/>
-      <c r="F81" s="35" t="s">
+      <c r="E81" s="35"/>
+      <c r="F81" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="G81" s="28" t="s">
+      <c r="G81" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A82" s="48"/>
-      <c r="B82" s="59"/>
-      <c r="C82" s="59"/>
-      <c r="D82" s="36" t="s">
+      <c r="A82" s="57"/>
+      <c r="B82" s="74"/>
+      <c r="C82" s="74"/>
+      <c r="D82" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="E82" s="36"/>
-      <c r="F82" s="35" t="s">
+      <c r="E82" s="35"/>
+      <c r="F82" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="G82" s="28" t="s">
+      <c r="G82" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A83" s="48"/>
-      <c r="B83" s="59"/>
-      <c r="C83" s="59"/>
-      <c r="D83" s="36" t="s">
+      <c r="A83" s="57"/>
+      <c r="B83" s="74"/>
+      <c r="C83" s="74"/>
+      <c r="D83" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="E83" s="36"/>
-      <c r="F83" s="35" t="s">
+      <c r="E83" s="35"/>
+      <c r="F83" s="34" t="s">
         <v>160</v>
       </c>
-      <c r="G83" s="28" t="s">
+      <c r="G83" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A84" s="48"/>
-      <c r="B84" s="59"/>
-      <c r="C84" s="59"/>
-      <c r="D84" s="36" t="s">
+      <c r="A84" s="57"/>
+      <c r="B84" s="74"/>
+      <c r="C84" s="74"/>
+      <c r="D84" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="E84" s="36"/>
-      <c r="F84" s="35" t="s">
+      <c r="E84" s="35"/>
+      <c r="F84" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="G84" s="28" t="s">
+      <c r="G84" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A85" s="48"/>
-      <c r="B85" s="59"/>
-      <c r="C85" s="59"/>
-      <c r="D85" s="36" t="s">
+      <c r="A85" s="57"/>
+      <c r="B85" s="74"/>
+      <c r="C85" s="74"/>
+      <c r="D85" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="E85" s="36"/>
-      <c r="F85" s="35" t="s">
+      <c r="E85" s="35"/>
+      <c r="F85" s="34" t="s">
         <v>162</v>
       </c>
-      <c r="G85" s="28" t="s">
+      <c r="G85" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A86" s="48"/>
-      <c r="B86" s="59"/>
-      <c r="C86" s="59"/>
-      <c r="D86" s="36" t="s">
+      <c r="A86" s="57"/>
+      <c r="B86" s="74"/>
+      <c r="C86" s="74"/>
+      <c r="D86" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="E86" s="36"/>
-      <c r="F86" s="35" t="s">
+      <c r="E86" s="35"/>
+      <c r="F86" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="G86" s="28" t="s">
+      <c r="G86" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A87" s="48"/>
-      <c r="B87" s="59"/>
-      <c r="C87" s="59"/>
-      <c r="D87" s="36" t="s">
+      <c r="A87" s="57"/>
+      <c r="B87" s="74"/>
+      <c r="C87" s="74"/>
+      <c r="D87" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="E87" s="36"/>
-      <c r="F87" s="35" t="s">
+      <c r="E87" s="35"/>
+      <c r="F87" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="G87" s="28" t="s">
+      <c r="G87" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A88" s="48"/>
-      <c r="B88" s="59"/>
-      <c r="C88" s="51" t="s">
+      <c r="A88" s="57"/>
+      <c r="B88" s="74"/>
+      <c r="C88" s="75" t="s">
         <v>181</v>
       </c>
-      <c r="D88" s="36" t="s">
+      <c r="D88" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="E88" s="36"/>
-      <c r="F88" s="35" t="s">
+      <c r="E88" s="35"/>
+      <c r="F88" s="34" t="s">
         <v>165</v>
       </c>
-      <c r="G88" s="28" t="s">
+      <c r="G88" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A89" s="48"/>
-      <c r="B89" s="59"/>
-      <c r="C89" s="51"/>
-      <c r="D89" s="36" t="s">
+      <c r="A89" s="57"/>
+      <c r="B89" s="74"/>
+      <c r="C89" s="75"/>
+      <c r="D89" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="E89" s="36"/>
-      <c r="F89" s="35" t="s">
+      <c r="E89" s="35"/>
+      <c r="F89" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="G89" s="28" t="s">
+      <c r="G89" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A90" s="48"/>
-      <c r="B90" s="59"/>
-      <c r="C90" s="51"/>
-      <c r="D90" s="36" t="s">
+      <c r="A90" s="57"/>
+      <c r="B90" s="74"/>
+      <c r="C90" s="75"/>
+      <c r="D90" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="E90" s="36"/>
-      <c r="F90" s="35" t="s">
+      <c r="E90" s="35"/>
+      <c r="F90" s="34" t="s">
         <v>167</v>
       </c>
-      <c r="G90" s="28" t="s">
+      <c r="G90" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A91" s="48"/>
-      <c r="B91" s="59"/>
-      <c r="C91" s="51"/>
-      <c r="D91" s="36" t="s">
+      <c r="A91" s="57"/>
+      <c r="B91" s="74"/>
+      <c r="C91" s="75"/>
+      <c r="D91" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="E91" s="36"/>
-      <c r="F91" s="35" t="s">
+      <c r="E91" s="35"/>
+      <c r="F91" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="G91" s="28" t="s">
+      <c r="G91" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A92" s="48"/>
-      <c r="B92" s="59"/>
-      <c r="C92" s="51"/>
-      <c r="D92" s="36" t="s">
+      <c r="A92" s="57"/>
+      <c r="B92" s="74"/>
+      <c r="C92" s="75"/>
+      <c r="D92" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="E92" s="36"/>
-      <c r="F92" s="35" t="s">
+      <c r="E92" s="35"/>
+      <c r="F92" s="34" t="s">
         <v>169</v>
       </c>
-      <c r="G92" s="28" t="s">
+      <c r="G92" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A93" s="48"/>
-      <c r="B93" s="59"/>
-      <c r="C93" s="51"/>
-      <c r="D93" s="36" t="s">
+      <c r="A93" s="57"/>
+      <c r="B93" s="74"/>
+      <c r="C93" s="75"/>
+      <c r="D93" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="E93" s="36"/>
-      <c r="F93" s="35" t="s">
+      <c r="E93" s="35"/>
+      <c r="F93" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="G93" s="28" t="s">
+      <c r="G93" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A94" s="48"/>
-      <c r="B94" s="59"/>
-      <c r="C94" s="51"/>
-      <c r="D94" s="36" t="s">
+      <c r="A94" s="57"/>
+      <c r="B94" s="74"/>
+      <c r="C94" s="75"/>
+      <c r="D94" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="E94" s="36"/>
-      <c r="F94" s="35" t="s">
+      <c r="E94" s="35"/>
+      <c r="F94" s="34" t="s">
         <v>171</v>
       </c>
-      <c r="G94" s="28" t="s">
+      <c r="G94" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A95" s="48"/>
-      <c r="B95" s="59"/>
-      <c r="C95" s="51" t="s">
+      <c r="A95" s="57"/>
+      <c r="B95" s="74"/>
+      <c r="C95" s="75" t="s">
         <v>172</v>
       </c>
-      <c r="D95" s="36" t="s">
+      <c r="D95" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="E95" s="36"/>
-      <c r="F95" s="35" t="s">
+      <c r="E95" s="35"/>
+      <c r="F95" s="34" t="s">
         <v>173</v>
       </c>
-      <c r="G95" s="28" t="s">
+      <c r="G95" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A96" s="48"/>
-      <c r="B96" s="59"/>
-      <c r="C96" s="51"/>
-      <c r="D96" s="36" t="s">
+      <c r="A96" s="57"/>
+      <c r="B96" s="74"/>
+      <c r="C96" s="75"/>
+      <c r="D96" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="E96" s="36"/>
-      <c r="F96" s="35" t="s">
+      <c r="E96" s="35"/>
+      <c r="F96" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="G96" s="28" t="s">
+      <c r="G96" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A97" s="48"/>
-      <c r="B97" s="59"/>
-      <c r="C97" s="51"/>
-      <c r="D97" s="36" t="s">
+      <c r="A97" s="57"/>
+      <c r="B97" s="74"/>
+      <c r="C97" s="75"/>
+      <c r="D97" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="E97" s="36"/>
-      <c r="F97" s="35" t="s">
+      <c r="E97" s="35"/>
+      <c r="F97" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="G97" s="28" t="s">
+      <c r="G97" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A98" s="48"/>
-      <c r="B98" s="59"/>
-      <c r="C98" s="51"/>
-      <c r="D98" s="36" t="s">
+      <c r="A98" s="57"/>
+      <c r="B98" s="74"/>
+      <c r="C98" s="75"/>
+      <c r="D98" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="E98" s="36"/>
-      <c r="F98" s="35" t="s">
+      <c r="E98" s="35"/>
+      <c r="F98" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="G98" s="28" t="s">
+      <c r="G98" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A99" s="48"/>
-      <c r="B99" s="59"/>
-      <c r="C99" s="51"/>
-      <c r="D99" s="36" t="s">
+      <c r="A99" s="57"/>
+      <c r="B99" s="74"/>
+      <c r="C99" s="75"/>
+      <c r="D99" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="E99" s="36"/>
-      <c r="F99" s="35" t="s">
+      <c r="E99" s="35"/>
+      <c r="F99" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="G99" s="28" t="s">
+      <c r="G99" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A100" s="48"/>
-      <c r="B100" s="59"/>
-      <c r="C100" s="51"/>
-      <c r="D100" s="36" t="s">
+      <c r="A100" s="57"/>
+      <c r="B100" s="74"/>
+      <c r="C100" s="75"/>
+      <c r="D100" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="E100" s="36"/>
-      <c r="F100" s="35" t="s">
+      <c r="E100" s="35"/>
+      <c r="F100" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="G100" s="28" t="s">
+      <c r="G100" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A101" s="48"/>
-      <c r="B101" s="59"/>
-      <c r="C101" s="51"/>
-      <c r="D101" s="36" t="s">
+      <c r="A101" s="57"/>
+      <c r="B101" s="74"/>
+      <c r="C101" s="75"/>
+      <c r="D101" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="E101" s="36"/>
-      <c r="F101" s="35" t="s">
+      <c r="E101" s="35"/>
+      <c r="F101" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="G101" s="28" t="s">
+      <c r="G101" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="48"/>
-      <c r="B102" s="59"/>
-      <c r="C102" s="59" t="s">
+      <c r="A102" s="57"/>
+      <c r="B102" s="74"/>
+      <c r="C102" s="74" t="s">
         <v>180</v>
       </c>
-      <c r="D102" s="36" t="s">
+      <c r="D102" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="E102" s="36"/>
-      <c r="F102" s="35" t="s">
+      <c r="E102" s="35"/>
+      <c r="F102" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="G102" s="28" t="s">
+      <c r="G102" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A103" s="48"/>
-      <c r="B103" s="59"/>
-      <c r="C103" s="59"/>
-      <c r="D103" s="36" t="s">
+      <c r="A103" s="57"/>
+      <c r="B103" s="74"/>
+      <c r="C103" s="74"/>
+      <c r="D103" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="E103" s="36"/>
-      <c r="F103" s="35" t="s">
+      <c r="E103" s="35"/>
+      <c r="F103" s="34" t="s">
         <v>184</v>
       </c>
-      <c r="G103" s="28" t="s">
+      <c r="G103" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A104" s="48"/>
-      <c r="B104" s="59"/>
-      <c r="C104" s="59"/>
-      <c r="D104" s="36" t="s">
+      <c r="A104" s="57"/>
+      <c r="B104" s="74"/>
+      <c r="C104" s="74"/>
+      <c r="D104" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="E104" s="36"/>
-      <c r="F104" s="35" t="s">
+      <c r="E104" s="35"/>
+      <c r="F104" s="34" t="s">
         <v>185</v>
       </c>
-      <c r="G104" s="28" t="s">
+      <c r="G104" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A105" s="48"/>
-      <c r="B105" s="59"/>
-      <c r="C105" s="59"/>
-      <c r="D105" s="36" t="s">
+      <c r="A105" s="57"/>
+      <c r="B105" s="74"/>
+      <c r="C105" s="74"/>
+      <c r="D105" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="E105" s="36"/>
-      <c r="F105" s="35" t="s">
+      <c r="E105" s="35"/>
+      <c r="F105" s="34" t="s">
         <v>186</v>
       </c>
-      <c r="G105" s="28" t="s">
+      <c r="G105" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A106" s="48"/>
-      <c r="B106" s="59"/>
-      <c r="C106" s="59"/>
-      <c r="D106" s="36" t="s">
+      <c r="A106" s="57"/>
+      <c r="B106" s="74"/>
+      <c r="C106" s="74"/>
+      <c r="D106" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="E106" s="36"/>
-      <c r="F106" s="35" t="s">
+      <c r="E106" s="35"/>
+      <c r="F106" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="G106" s="28" t="s">
+      <c r="G106" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A107" s="48"/>
-      <c r="B107" s="59"/>
-      <c r="C107" s="59"/>
-      <c r="D107" s="36" t="s">
+      <c r="A107" s="57"/>
+      <c r="B107" s="74"/>
+      <c r="C107" s="74"/>
+      <c r="D107" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="E107" s="36"/>
-      <c r="F107" s="35" t="s">
+      <c r="E107" s="35"/>
+      <c r="F107" s="34" t="s">
         <v>188</v>
       </c>
-      <c r="G107" s="28" t="s">
+      <c r="G107" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A108" s="48"/>
-      <c r="B108" s="59"/>
-      <c r="C108" s="59"/>
-      <c r="D108" s="36" t="s">
+      <c r="A108" s="57"/>
+      <c r="B108" s="74"/>
+      <c r="C108" s="74"/>
+      <c r="D108" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="E108" s="36"/>
-      <c r="F108" s="35" t="s">
+      <c r="E108" s="35"/>
+      <c r="F108" s="34" t="s">
         <v>189</v>
       </c>
-      <c r="G108" s="28" t="s">
+      <c r="G108" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A109" s="48"/>
-      <c r="B109" s="59"/>
-      <c r="C109" s="51" t="s">
+      <c r="A109" s="57"/>
+      <c r="B109" s="74"/>
+      <c r="C109" s="75" t="s">
         <v>190</v>
       </c>
-      <c r="D109" s="36" t="s">
+      <c r="D109" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="E109" s="36"/>
-      <c r="F109" s="35" t="s">
+      <c r="E109" s="35"/>
+      <c r="F109" s="34" t="s">
         <v>191</v>
       </c>
-      <c r="G109" s="28" t="s">
+      <c r="G109" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A110" s="48"/>
-      <c r="B110" s="59"/>
-      <c r="C110" s="51"/>
-      <c r="D110" s="36" t="s">
+      <c r="A110" s="57"/>
+      <c r="B110" s="74"/>
+      <c r="C110" s="75"/>
+      <c r="D110" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="E110" s="36"/>
-      <c r="F110" s="35" t="s">
+      <c r="E110" s="35"/>
+      <c r="F110" s="34" t="s">
         <v>192</v>
       </c>
-      <c r="G110" s="28" t="s">
+      <c r="G110" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A111" s="48"/>
-      <c r="B111" s="59"/>
-      <c r="C111" s="51"/>
-      <c r="D111" s="36" t="s">
+      <c r="A111" s="57"/>
+      <c r="B111" s="74"/>
+      <c r="C111" s="75"/>
+      <c r="D111" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="E111" s="36"/>
-      <c r="F111" s="35" t="s">
+      <c r="E111" s="35"/>
+      <c r="F111" s="34" t="s">
         <v>193</v>
       </c>
-      <c r="G111" s="28" t="s">
+      <c r="G111" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A112" s="48"/>
-      <c r="B112" s="59"/>
-      <c r="C112" s="51"/>
-      <c r="D112" s="36" t="s">
+      <c r="A112" s="57"/>
+      <c r="B112" s="74"/>
+      <c r="C112" s="75"/>
+      <c r="D112" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="E112" s="36"/>
-      <c r="F112" s="35" t="s">
+      <c r="E112" s="35"/>
+      <c r="F112" s="34" t="s">
         <v>194</v>
       </c>
-      <c r="G112" s="28" t="s">
+      <c r="G112" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A113" s="48"/>
-      <c r="B113" s="59"/>
-      <c r="C113" s="51"/>
-      <c r="D113" s="36" t="s">
+      <c r="A113" s="57"/>
+      <c r="B113" s="74"/>
+      <c r="C113" s="75"/>
+      <c r="D113" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="E113" s="36"/>
-      <c r="F113" s="35" t="s">
+      <c r="E113" s="35"/>
+      <c r="F113" s="34" t="s">
         <v>195</v>
       </c>
-      <c r="G113" s="28" t="s">
+      <c r="G113" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A114" s="48"/>
-      <c r="B114" s="59"/>
-      <c r="C114" s="51"/>
-      <c r="D114" s="36" t="s">
+      <c r="A114" s="57"/>
+      <c r="B114" s="74"/>
+      <c r="C114" s="75"/>
+      <c r="D114" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="E114" s="36"/>
-      <c r="F114" s="35" t="s">
+      <c r="E114" s="35"/>
+      <c r="F114" s="34" t="s">
         <v>196</v>
       </c>
-      <c r="G114" s="28" t="s">
+      <c r="G114" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A115" s="48"/>
-      <c r="B115" s="59"/>
-      <c r="C115" s="51"/>
-      <c r="D115" s="36" t="s">
+      <c r="A115" s="57"/>
+      <c r="B115" s="74"/>
+      <c r="C115" s="75"/>
+      <c r="D115" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="E115" s="36"/>
-      <c r="F115" s="35" t="s">
+      <c r="E115" s="35"/>
+      <c r="F115" s="34" t="s">
         <v>197</v>
       </c>
-      <c r="G115" s="28" t="s">
+      <c r="G115" s="27" t="s">
         <v>214</v>
       </c>
     </row>
@@ -3472,72 +3479,125 @@
       <c r="A116" s="58" t="s">
         <v>198</v>
       </c>
-      <c r="B116" s="49" t="s">
+      <c r="B116" s="73" t="s">
         <v>199</v>
       </c>
-      <c r="C116" s="49"/>
-      <c r="D116" s="49"/>
-      <c r="E116" s="37"/>
-      <c r="F116" s="9" t="s">
+      <c r="C116" s="73"/>
+      <c r="D116" s="73"/>
+      <c r="E116" s="44"/>
+      <c r="F116" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="G116" s="29" t="s">
+      <c r="G116" s="28" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" s="58"/>
-      <c r="B117" s="47" t="s">
+      <c r="B117" s="77" t="s">
         <v>201</v>
       </c>
-      <c r="C117" s="49"/>
-      <c r="D117" s="49"/>
-      <c r="E117" s="37"/>
-      <c r="F117" s="9" t="s">
+      <c r="C117" s="73"/>
+      <c r="D117" s="73"/>
+      <c r="E117" s="44"/>
+      <c r="F117" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="G117" s="29" t="s">
+      <c r="G117" s="28" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="58"/>
-      <c r="B118" s="47" t="s">
+      <c r="B118" s="77" t="s">
         <v>205</v>
       </c>
-      <c r="C118" s="47"/>
-      <c r="D118" s="47"/>
-      <c r="E118" s="38"/>
-      <c r="F118" s="9" t="s">
+      <c r="C118" s="77"/>
+      <c r="D118" s="77"/>
+      <c r="E118" s="43"/>
+      <c r="F118" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="G118" s="29" t="s">
+      <c r="G118" s="28" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" s="58"/>
-      <c r="B119" s="49" t="s">
+      <c r="B119" s="73" t="s">
         <v>203</v>
       </c>
-      <c r="C119" s="49"/>
-      <c r="D119" s="49"/>
-      <c r="E119" s="37"/>
-      <c r="F119" s="9" t="s">
+      <c r="C119" s="73"/>
+      <c r="D119" s="73"/>
+      <c r="E119" s="44"/>
+      <c r="F119" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="G119" s="29" t="s">
+      <c r="G119" s="28" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B120" s="2"/>
-      <c r="C120" s="2"/>
-      <c r="D120" s="2"/>
-      <c r="E120" s="2"/>
+      <c r="A120" s="58"/>
+      <c r="B120" s="73" t="s">
+        <v>287</v>
+      </c>
+      <c r="C120" s="73"/>
+      <c r="D120" s="73"/>
+      <c r="E120" s="81"/>
+      <c r="F120" s="82" t="s">
+        <v>286</v>
+      </c>
+      <c r="G120" s="28" t="s">
+        <v>222</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="59">
+  <mergeCells count="60">
+    <mergeCell ref="B120:D120"/>
+    <mergeCell ref="A116:A120"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B118:D118"/>
+    <mergeCell ref="A58:A115"/>
+    <mergeCell ref="B116:D116"/>
+    <mergeCell ref="B117:D117"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="C60:C66"/>
+    <mergeCell ref="C67:C73"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B46:C49"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E46:E49"/>
+    <mergeCell ref="B119:D119"/>
+    <mergeCell ref="C74:C80"/>
+    <mergeCell ref="C81:C87"/>
+    <mergeCell ref="C88:C94"/>
+    <mergeCell ref="C95:C101"/>
+    <mergeCell ref="C102:C108"/>
+    <mergeCell ref="C109:C115"/>
+    <mergeCell ref="B60:B115"/>
+    <mergeCell ref="A46:A57"/>
+    <mergeCell ref="B25:C29"/>
+    <mergeCell ref="B30:C34"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B50:C57"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B41:C43"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="B20:C24"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="B38:D38"/>
     <mergeCell ref="B35:D35"/>
@@ -3554,49 +3614,6 @@
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="B20:C24"/>
-    <mergeCell ref="B25:C29"/>
-    <mergeCell ref="B30:C34"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B50:C57"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B41:C43"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="E46:E49"/>
-    <mergeCell ref="B119:D119"/>
-    <mergeCell ref="A116:A119"/>
-    <mergeCell ref="C74:C80"/>
-    <mergeCell ref="C81:C87"/>
-    <mergeCell ref="C88:C94"/>
-    <mergeCell ref="C95:C101"/>
-    <mergeCell ref="C102:C108"/>
-    <mergeCell ref="C109:C115"/>
-    <mergeCell ref="B60:B115"/>
-    <mergeCell ref="A46:A57"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B118:D118"/>
-    <mergeCell ref="A58:A115"/>
-    <mergeCell ref="B116:D116"/>
-    <mergeCell ref="B117:D117"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="C60:C66"/>
-    <mergeCell ref="C67:C73"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B46:C49"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3606,7 +3623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -3619,176 +3636,176 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="79" t="s">
         <v>223</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="37" t="s">
         <v>225</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="37" t="s">
         <v>224</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="37" t="s">
         <v>207</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="37" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="31" t="s">
         <v>246</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="39" t="s">
         <v>256</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="31" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="38" t="s">
         <v>226</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="39" t="s">
         <v>253</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="39" t="s">
         <v>258</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="31" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="38" t="s">
         <v>227</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="31" t="s">
         <v>228</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="31" t="s">
         <v>229</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="31" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="38" t="s">
         <v>248</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="31" t="s">
         <v>230</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="31" t="s">
         <v>229</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="31" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="31" t="s">
         <v>232</v>
       </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32" t="s">
+      <c r="C7" s="31"/>
+      <c r="D7" s="31" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="38" t="s">
         <v>233</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="39" t="s">
         <v>234</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="31" t="s">
         <v>285</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="31" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="38" t="s">
         <v>235</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="31" t="s">
         <v>236</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="31" t="s">
         <v>237</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="31" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="38" t="s">
         <v>247</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="31" t="s">
         <v>238</v>
       </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32" t="s">
+      <c r="C10" s="31"/>
+      <c r="D10" s="31" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="38" t="s">
         <v>239</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="39" t="s">
         <v>240</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="39" t="s">
         <v>258</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="31" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="192" x14ac:dyDescent="0.2">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="38" t="s">
         <v>241</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="31" t="s">
         <v>242</v>
       </c>
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="39" t="s">
         <v>255</v>
       </c>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="31" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="31" t="s">
         <v>244</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="31" t="s">
         <v>245</v>
       </c>
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="31" t="s">
         <v>252</v>
       </c>
     </row>
@@ -3817,154 +3834,154 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="80" t="s">
         <v>259</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="41" t="s">
         <v>225</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="41" t="s">
         <v>224</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="41" t="s">
         <v>207</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="41" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="39" t="s">
         <v>260</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="39" t="s">
         <v>261</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="31" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="39" t="s">
         <v>246</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="39" t="s">
         <v>256</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="39" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="42" t="s">
         <v>262</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="39" t="s">
         <v>267</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="39" t="s">
         <v>272</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="39" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="42" t="s">
         <v>264</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="39" t="s">
         <v>268</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42" t="s">
+      <c r="C6" s="39"/>
+      <c r="D6" s="39" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="42" t="s">
         <v>266</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42" t="s">
+      <c r="C7" s="39"/>
+      <c r="D7" s="39" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="42" t="s">
         <v>279</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="39" t="s">
         <v>280</v>
       </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42" t="s">
+      <c r="C8" s="39"/>
+      <c r="D8" s="39" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="42" t="s">
         <v>282</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="39" t="s">
         <v>283</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="39" t="s">
         <v>284</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="39" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="42" t="s">
         <v>271</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="39" t="s">
         <v>273</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="39" t="s">
         <v>272</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="39" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="42" t="s">
         <v>277</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="39" t="s">
         <v>278</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42" t="s">
+      <c r="C11" s="39"/>
+      <c r="D11" s="39" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="42" t="s">
         <v>274</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="39" t="s">
         <v>275</v>
       </c>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42" t="s">
+      <c r="C12" s="39"/>
+      <c r="D12" s="39" t="s">
         <v>276</v>
       </c>
     </row>

</xml_diff>